<commit_message>
Updated version after 12 April
</commit_message>
<xml_diff>
--- a/SpecimenCollectionForm/DB and Documents/Specimen Collection- Endline Parasite.xlsx
+++ b/SpecimenCollectionForm/DB and Documents/Specimen Collection- Endline Parasite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="2" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questions!$V$1:$V$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questions!$V$1:$V$55</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="231">
   <si>
     <t>SLNo</t>
   </si>
@@ -551,8 +551,203 @@
     <t>msg01</t>
   </si>
   <si>
+    <t>NOTE: Mark the cap of the stool collection containersin this household with * to show that this household is in the single arm EE cohort.</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>msg02</t>
+  </si>
+  <si>
+    <t>q13_other</t>
+  </si>
+  <si>
+    <t>q14_other</t>
+  </si>
+  <si>
+    <t>msg03</t>
+  </si>
+  <si>
+    <t>D³ Lvbvi Uv‡M©U wkï Ges Uv‡M©U wkïi RgR †_‡K i‡³i bgybv msMÖn Ki‡Z n‡ebv|</t>
+  </si>
+  <si>
+    <t>Do not collect a blood sample from target child (and twin) in this household</t>
+  </si>
+  <si>
+    <t>msg04</t>
+  </si>
+  <si>
+    <t>q19a</t>
+  </si>
+  <si>
+    <t>q19b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.‡hme e¨w³i KvQ †_‡K GLb bgybv msMÖn Kiv n‡”Q Zv‡`i cÖ‡Z¨‡Ki Avjv`v Avjv`v AvBwW wbev©Pb Kiæb  (GKwU AvBwW wbev©Pb Kiæb)    </t>
+  </si>
+  <si>
+    <t>6.Select the ID of the individual whose sample you are collecting now (select one)</t>
+  </si>
+  <si>
+    <t>7. Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)</t>
+  </si>
+  <si>
+    <t>7.Enter the name of the individual (check against your ID list from Day1 team)</t>
+  </si>
+  <si>
+    <t>1.cvqLvbv</t>
+  </si>
+  <si>
+    <t>1.Stool</t>
+  </si>
+  <si>
+    <t>1.GKev‡I Kiv cvqLvbv †_‡K</t>
+  </si>
+  <si>
+    <t>1.Single</t>
+  </si>
+  <si>
+    <t>2.GKvwaKev‡I Kiv cvqLvbv †_‡K</t>
+  </si>
+  <si>
+    <t>2.Multiple</t>
+  </si>
+  <si>
+    <t>q21_other</t>
+  </si>
+  <si>
+    <t>8.Are you collecting stool or bloodfrom this person right now?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wbwðZ Kiæb †h cvqLvbvi bgybv cixÿv Kivi Rb¨ Avcwb K¨v‡Uv-K¨vUR GwjKU ˆZix K‡i‡Qb Ges K¨v‡Uv-K¨vUR GwjK‡Ui Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q| </t>
+  </si>
+  <si>
+    <t>Make sure that you have prepared a Kato-Katz aliquot for this individual and make sure that the sample ID and random ID of the barcode on the Kato-Katz aliquot match the following:</t>
+  </si>
+  <si>
+    <t>11.msM„nxZ bgybv Kyje†· ivLvi ïiæi mgqUv wjwce× Kiæb (24 N›Uv wnmv‡e)</t>
+  </si>
+  <si>
+    <t>11.Enter the cold chain start time  (24-hr scale)</t>
+  </si>
+  <si>
+    <t>12.(পর্যবেক্ষন করুন) cvqLvbvi aib †Kgb?</t>
+  </si>
+  <si>
+    <t>12.(obs) Stool consistency</t>
+  </si>
+  <si>
+    <t>13.(পর্যবেক্ষন করুন) cvqLvbvi eb© wK?</t>
+  </si>
+  <si>
+    <t>13. (obs) Stool color</t>
+  </si>
+  <si>
+    <t>13.Ab¨vY¨t wbw`©ó K‡i wjLyb</t>
+  </si>
+  <si>
+    <t>13.Other: Specify</t>
+  </si>
+  <si>
+    <t>14. (পর্যবেক্ষন করুন) msM„nxZ cvqLvbvi bgybvi g‡a¨ A¯^vfvweK wKQz †`Lv †M‡Q wK? (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)</t>
+  </si>
+  <si>
+    <t>14.(obs) Do you see any abnormal characteristics of the collected stool sample? (Select all that apply)</t>
+  </si>
+  <si>
+    <t>14.Ab¨vY¨t wbw`©ó K‡i wjLyb</t>
+  </si>
+  <si>
+    <t>14.Other: Specify</t>
+  </si>
+  <si>
+    <t>15.Enter the day of defecation</t>
+  </si>
+  <si>
+    <t>16.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi mgq wjwce× Kiæb (24 N›Uv wnmv‡e, Rvwb bv n‡j 99:99 emvb)</t>
+  </si>
+  <si>
+    <t>16.Enter the time of defecation (24-hr scale, enter 99:99 for DK)</t>
+  </si>
+  <si>
+    <t>17.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb</t>
+  </si>
+  <si>
+    <t>17.Enter the approximate time of defecation</t>
+  </si>
+  <si>
+    <t>18.cvqLvbvi bgybvwU GKev‡I Kiv cvqLvbv †_‡K bvwKGKvwaKevi Kiv cvqLvbv †_‡K msMÖn Kiv n‡q‡Q?</t>
+  </si>
+  <si>
+    <t>18.Was the stool collected from one defecation event or multiple defecation events?</t>
+  </si>
+  <si>
+    <t>19.K.(পর্যবেক্ষন করুন) D³ e¨w³/wkï cv‡q RyZv c‡o‡Q wK ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.a. (obs) Is the individual wearing shoes? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.L.BB wUg D³ Uv‡M©U wkï (Ges Uv‡M©U wkïi RgR) †_‡K i‡³i bgybv msMÖn K‡i‡Q wK ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.b. Has a target child (and twin) blood sample already been collected by the EE team? </t>
+  </si>
+  <si>
+    <t>21.Ab¨vY¨t wbw`©ó K‡i wjLyb</t>
+  </si>
+  <si>
+    <t>21.Other: Specify</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22. A¨vwbwgqv †U‡÷i djvdj wjLyb </t>
+  </si>
+  <si>
+    <t>22.Enter the result of the anemia test. __ __. __ g/dL</t>
+  </si>
+  <si>
+    <t>wbwðZ Kiæb eøvW ¯úU wdëvi †ccv‡ii Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q|</t>
+  </si>
+  <si>
+    <t>Make sure that the sample ID and random ID of the barcode on the blood spot filter paper match the following:</t>
+  </si>
+  <si>
+    <t>8.Avcwb wK GLb D³ e¨w³ †_‡K cvqLvbv ev i‡³i bgybv msMÖn Ki‡eb?</t>
+  </si>
+  <si>
+    <t>q10_other</t>
+  </si>
+  <si>
+    <t>10.Ab¨vY¨t wbw`©ó K‡i wjLyb</t>
+  </si>
+  <si>
+    <t>10.Other: Specify</t>
+  </si>
+  <si>
+    <t>qSpil</t>
+  </si>
+  <si>
+    <t>20.Has a blood sample been collected from this individual?</t>
+  </si>
+  <si>
+    <t>Is this a spillover household?</t>
+  </si>
+  <si>
+    <t>GUv wK w¯cjIfvi nvDR‡nvì?</t>
+  </si>
+  <si>
+    <t>3.i‡³i bgybv</t>
+  </si>
+  <si>
+    <t>2.cvqLvbv + i‡³i bgybv</t>
+  </si>
+  <si>
+    <t>2.Stool and blood</t>
+  </si>
+  <si>
     <r>
-      <t>D³ LvbvwUbZzb BB wm‡½j Av‡g©i AšÍ©fz³ wn‡m‡e wb‡`©k Ki‡Zev †evSv‡ZmsMÖnK…Z ÷zj K‡›UBbv‡ii wQwci Dci ZviKv wPý (</t>
+      <t>D³ LvbvwU bZzb BB wm‡½j Av‡g©i AšÍ©fz³ wn‡m‡e wb‡`©k Ki‡Z ev †evSv‡Z msMÖnK…Z ÷zj K‡›UBbv‡ii wQwci Dci ZviKv wPý (</t>
     </r>
     <r>
       <rPr>
@@ -574,208 +769,25 @@
     </r>
   </si>
   <si>
-    <t>NOTE: Mark the cap of the stool collection containersin this household with * to show that this household is in the single arm EE cohort.</t>
-  </si>
-  <si>
-    <t>q6</t>
-  </si>
-  <si>
-    <t>msg02</t>
-  </si>
-  <si>
-    <t>q13_other</t>
-  </si>
-  <si>
-    <t>q14_other</t>
-  </si>
-  <si>
-    <t>msg03</t>
-  </si>
-  <si>
-    <t>D³ Lvbvi Uv‡M©U wkï Ges Uv‡M©U wkïi RgR †_‡K i‡³i bgybv msMÖn Ki‡Z n‡ebv|</t>
-  </si>
-  <si>
-    <t>Do not collect a blood sample from target child (and twin) in this household</t>
-  </si>
-  <si>
-    <t>msg04</t>
-  </si>
-  <si>
-    <t>q19a</t>
-  </si>
-  <si>
-    <t>q19b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.‡hme e¨w³i KvQ †_‡K GLb bgybv msMÖn Kiv n‡”Q Zv‡`i cÖ‡Z¨‡Ki Avjv`v Avjv`v AvBwW wbev©Pb Kiæb  (GKwU AvBwW wbev©Pb Kiæb)    </t>
-  </si>
-  <si>
-    <t>6.Select the ID of the individual whose sample you are collecting now (select one)</t>
-  </si>
-  <si>
-    <t>7. Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)</t>
-  </si>
-  <si>
-    <t>7.Enter the name of the individual (check against your ID list from Day1 team)</t>
-  </si>
-  <si>
-    <t>1.cvqLvbv</t>
-  </si>
-  <si>
-    <t>1.Stool</t>
-  </si>
-  <si>
-    <t>2.i‡³i bgybv</t>
-  </si>
-  <si>
-    <t>2.Blood</t>
-  </si>
-  <si>
-    <t>1.GKev‡I Kiv cvqLvbv †_‡K</t>
-  </si>
-  <si>
-    <t>1.Single</t>
-  </si>
-  <si>
-    <t>2.GKvwaKev‡I Kiv cvqLvbv †_‡K</t>
-  </si>
-  <si>
-    <t>2.Multiple</t>
-  </si>
-  <si>
-    <t>q21_other</t>
-  </si>
-  <si>
-    <t>8.Are you collecting stool or bloodfrom this person right now?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wbwðZ Kiæb †h cvqLvbvi bgybv cixÿv Kivi Rb¨ Avcwb K¨v‡Uv-K¨vUR GwjKU ˆZix K‡i‡Qb Ges K¨v‡Uv-K¨vUR GwjK‡Ui Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q| </t>
-  </si>
-  <si>
-    <t>Make sure that you have prepared a Kato-Katz aliquot for this individual and make sure that the sample ID and random ID of the barcode on the Kato-Katz aliquot match the following:</t>
-  </si>
-  <si>
-    <t>11.msM„nxZ bgybv Kyje†· ivLvi ïiæi mgqUv wjwce× Kiæb (24 N›Uv wnmv‡e)</t>
-  </si>
-  <si>
-    <t>11.Enter the cold chain start time  (24-hr scale)</t>
-  </si>
-  <si>
-    <t>12.(পর্যবেক্ষন করুন) cvqLvbvi aib †Kgb?</t>
-  </si>
-  <si>
-    <t>12.(obs) Stool consistency</t>
-  </si>
-  <si>
-    <t>13.(পর্যবেক্ষন করুন) cvqLvbvi eb© wK?</t>
-  </si>
-  <si>
-    <t>13. (obs) Stool color</t>
-  </si>
-  <si>
-    <t>13.Ab¨vY¨t wbw`©ó K‡i wjLyb</t>
-  </si>
-  <si>
-    <t>13.Other: Specify</t>
-  </si>
-  <si>
-    <t>14. (পর্যবেক্ষন করুন) msM„nxZ cvqLvbvi bgybvi g‡a¨ A¯^vfvweK wKQz †`Lv †M‡Q wK? (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)</t>
-  </si>
-  <si>
-    <t>14.(obs) Do you see any abnormal characteristics of the collected stool sample? (Select all that apply)</t>
-  </si>
-  <si>
-    <t>14.Ab¨vY¨t wbw`©ó K‡i wjLyb</t>
-  </si>
-  <si>
-    <t>14.Other: Specify</t>
-  </si>
-  <si>
-    <t>15.Enter the day of defecation</t>
-  </si>
-  <si>
-    <t>16.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi mgq wjwce× Kiæb (24 N›Uv wnmv‡e, Rvwb bv n‡j 99:99 emvb)</t>
-  </si>
-  <si>
-    <t>16.Enter the time of defecation (24-hr scale, enter 99:99 for DK)</t>
-  </si>
-  <si>
-    <t>17.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb</t>
-  </si>
-  <si>
-    <t>17.Enter the approximate time of defecation</t>
-  </si>
-  <si>
-    <t>18.cvqLvbvi bgybvwU GKev‡I Kiv cvqLvbv †_‡K bvwKGKvwaKevi Kiv cvqLvbv †_‡K msMÖn Kiv n‡q‡Q?</t>
-  </si>
-  <si>
-    <t>18.Was the stool collected from one defecation event or multiple defecation events?</t>
-  </si>
-  <si>
-    <t>19.K.(পর্যবেক্ষন করুন) D³ e¨w³/wkï cv‡q RyZv c‡o‡Q wK ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.a. (obs) Is the individual wearing shoes? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.L.BB wUg D³ Uv‡M©U wkï (Ges Uv‡M©U wkïi RgR) †_‡K i‡³i bgybv msMÖn K‡i‡Q wK ? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.b. Has a target child (and twin) blood sample already been collected by the EE team? </t>
-  </si>
-  <si>
-    <t>21.Ab¨vY¨t wbw`©ó K‡i wjLyb</t>
-  </si>
-  <si>
-    <t>21.Other: Specify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22. A¨vwbwgqv †U‡÷i djvdj wjLyb </t>
-  </si>
-  <si>
-    <t>22.Enter the result of the anemia test. __ __. __ g/dL</t>
-  </si>
-  <si>
-    <t>wbwðZ Kiæb eøvW ¯úU wdëvi †ccv‡ii Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q|</t>
-  </si>
-  <si>
-    <t>Make sure that the sample ID and random ID of the barcode on the blood spot filter paper match the following:</t>
-  </si>
-  <si>
-    <t>8.Avcwb wK GLb D³ e¨w³ †_‡K cvqLvbv ev i‡³i bgybv msMÖn Ki‡eb?</t>
-  </si>
-  <si>
-    <t>q10_other</t>
-  </si>
-  <si>
-    <t>10.Ab¨vY¨t wbw`©ó K‡i wjLyb</t>
-  </si>
-  <si>
-    <t>10.Other: Specify</t>
-  </si>
-  <si>
-    <t>w¯cj Ifvi AvBwW Av‡Q?</t>
-  </si>
-  <si>
-    <t>Spillover ID aviailable?</t>
-  </si>
-  <si>
-    <t>qspilid</t>
-  </si>
-  <si>
-    <t>w¯cj Ifvi AvBwW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spillover ID </t>
-  </si>
-  <si>
-    <t>qSpil</t>
-  </si>
-  <si>
-    <t>qSpilid</t>
-  </si>
-  <si>
-    <t>20.Has a blood sample been collected from this individual?</t>
+    <t>3.ch©‡eÿb Kiv m¤¢e nqwb</t>
+  </si>
+  <si>
+    <t>3.Could not observe</t>
+  </si>
+  <si>
+    <t>q14_1</t>
+  </si>
+  <si>
+    <t>q14_2</t>
+  </si>
+  <si>
+    <t>q14_3</t>
+  </si>
+  <si>
+    <t>q14_4</t>
+  </si>
+  <si>
+    <t>q14_5</t>
   </si>
 </sst>
 </file>
@@ -1675,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DK441"/>
+  <dimension ref="A1:DK440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="Q29" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1854,109 +1866,118 @@
       <c r="DJ1" s="16"/>
       <c r="DK1" s="16"/>
     </row>
-    <row r="2" spans="1:115" ht="75">
+    <row r="2" spans="1:115" s="40" customFormat="1" ht="75">
       <c r="A2" s="29">
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>26</v>
+        <v>216</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>36</v>
+        <v>219</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>37</v>
+        <v>218</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="S2" s="39" t="s">
+      <c r="S2" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="T2" s="39" t="s">
+      <c r="T2" s="40" t="s">
         <v>127</v>
       </c>
       <c r="V2" s="22" t="str">
         <f>"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A2&amp;"', '" &amp;B2&amp;"','" &amp;C2&amp;"', '" &amp;D2&amp;"','" &amp;E2&amp;"','" &amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"', '"&amp;K2&amp;"','"&amp;L2&amp;"','"&amp;M2&amp;"','"&amp;N2&amp;"','"&amp;O2&amp;"','"&amp;P2&amp;"','"&amp;Q2&amp;"',"&amp;R2&amp;","&amp;S2&amp;",'"&amp;T2&amp;"');"</f>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('1', 'dataid','frmdataid', 'tblMainQues','1-2.K¬v÷vi AvBwW I gv‡qi  AvBwW','1-2.Cluster ID and  Mother ID ','','qSpil','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:115" s="40" customFormat="1" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('1', 'qSpil','frmsinglechoice', 'tblMainQues','GUv wK w¯cjIfvi nvDR‡nvì?','Is this a spillover household?','','dataid','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:115" ht="90">
       <c r="A3" s="29">
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>224</v>
+        <v>26</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>219</v>
+        <v>36</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>220</v>
+        <v>37</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="R3" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="T3" s="40" t="s">
+      <c r="T3" s="39" t="s">
         <v>127</v>
       </c>
       <c r="V3" s="22" t="str">
-        <f t="shared" ref="V3:V34" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'qSpil','frmsinglechoice', 'tblMainQues','w¯cj Ifvi AvBwW Av‡Q?','Spillover ID aviailable?','','qSpilid','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:115" s="40" customFormat="1" ht="75">
+        <f t="shared" ref="V3:V33" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'dataid','frmdataid', 'tblMainQues','1-2.K¬v÷vi AvBwW I gv‡qi  AvBwW','1-2.Cluster ID and  Mother ID ','','q3','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:115" ht="90">
       <c r="A4" s="29">
         <v>3</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>225</v>
+        <v>31</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>223</v>
+        <v>155</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>38</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
       <c r="R4" s="40" t="s">
         <v>126</v>
       </c>
@@ -1966,32 +1987,33 @@
       <c r="T4" s="40" t="s">
         <v>127</v>
       </c>
+      <c r="U4" s="40"/>
       <c r="V4" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('3', 'qSpilid','frmnumeric', 'tblMainQues','w¯cj Ifvi AvBwW','Spillover ID ','','q3','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:115" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('3', 'q3','frmcombobox', 'tblMainQues','3.bgybv msMÖnKvixi AvBwW I bvg (ZvwjKv †_‡K GKRb‡K wbev©Pb Kiæb) ','3. MT ID and name (select one)  ','','q4','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:115" ht="90.75">
       <c r="A5" s="29">
         <v>4</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>155</v>
+      <c r="E5" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2014,30 +2036,30 @@
       <c r="U5" s="40"/>
       <c r="V5" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'q3','frmcombobox', 'tblMainQues','3.bgybv msMÖnKvixi AvBwW I bvg (ZvwjKv †_‡K GKRb‡K wbev©Pb Kiæb) ','3. MT ID and name (select one)  ','','q4','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:115" ht="75.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'q4','frmdate', 'tblMainQues','4.bgybv msMÖ‡ni ZvwiL ','4. Data of sample collection ','','q5','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:115" ht="94.5">
       <c r="A6" s="29">
         <v>5</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>39</v>
+      <c r="E6" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -2060,30 +2082,30 @@
       <c r="U6" s="40"/>
       <c r="V6" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('5', 'q4','frmdate', 'tblMainQues','4.bgybv msMÖ‡ni ZvwiL ','4. Data of sample collection ','','q5','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:115" ht="94.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('5', 'q5','frmmultiplechoice', 'tblMainQues','5.†h wkï †_‡K bgybv msMÖ‡ni Rb¨ cÖ_g w`b ÷zj K‡›UBbvi †`Iqv n‡q‡Q Zvi AvBwW wbev©Pb Kiæb (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','5. Select which children have been given stool container on Day1 (select all that apply)','','q6','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:115" ht="99">
       <c r="A7" s="29">
         <v>6</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>41</v>
+        <v>143</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>169</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>157</v>
+        <v>43</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -2106,31 +2128,40 @@
       <c r="U7" s="40"/>
       <c r="V7" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('6', 'q5','frmmultiplechoice', 'tblMainQues','5.†h wkï †_‡K bgybv msMÖ‡ni Rb¨ cÖ_g w`b ÷zj K‡›UBbvi †`Iqv n‡q‡Q Zvi AvBwW wbev©Pb Kiæb (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','5. Select which children have been given stool container on Day1 (select all that apply)','','msg01','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:115" s="40" customFormat="1" ht="105">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('6', 'q6','frmcombobox', 'tblMainQuesL','6.‡hme e¨w³i KvQ †_‡K GLb bgybv msMÖn Kiv n‡”Q Zv‡`i cÖ‡Z¨‡Ki Avjv`v Avjv`v AvBwW wbev©Pb Kiæb  (GKwU AvBwW wbev©Pb Kiæb)    ','6.Select the ID of the individual whose sample you are collecting now (select one)','','q7','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:115" ht="90">
       <c r="A8" s="29">
         <v>7</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>156</v>
+        <v>43</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>158</v>
+        <v>143</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>171</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>160</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
       <c r="R8" s="40" t="s">
         <v>126</v>
       </c>
@@ -2140,42 +2171,34 @@
       <c r="T8" s="40" t="s">
         <v>127</v>
       </c>
+      <c r="U8" s="40"/>
       <c r="V8" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'msg01','frmmessage', 'tblMainQues','D³ LvbvwUbZzb BB wm‡½j Av‡g©i AšÍ©fz³ wn‡m‡e wb‡`©k Ki‡Zev †evSv‡ZmsMÖnK…Z ÷zj K‡›UBbv‡ii wQwci Dci ZviKv wPý (*) emvb','NOTE: Mark the cap of the stool collection containersin this household with * to show that this household is in the single arm EE cohort.','','q6','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:115" ht="99">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'q7','frmtext', 'tblMainQuesL','7. Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)','7.Enter the name of the individual (check against your ID list from Day1 team)','','q8','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:115" s="40" customFormat="1" ht="90.75">
       <c r="A9" s="29">
         <v>8</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>171</v>
+      <c r="E9" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>180</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
+        <v>50</v>
+      </c>
       <c r="R9" s="40" t="s">
         <v>126</v>
       </c>
@@ -2185,33 +2208,32 @@
       <c r="T9" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="U9" s="40"/>
       <c r="V9" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'q6','frmcombobox', 'tblMainQuesL','6.‡hme e¨w³i KvQ †_‡K GLb bgybv msMÖn Kiv n‡”Q Zv‡`i cÖ‡Z¨‡Ki Avjv`v Avjv`v AvBwW wbev©Pb Kiæb  (GKwU AvBwW wbev©Pb Kiæb)    ','6.Select the ID of the individual whose sample you are collecting now (select one)','','q7','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:115" ht="78.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'q8','frmsinglechoice', 'tblMainQuesL','8.Avcwb wK GLb D³ e¨w³ †_‡K cvqLvbv ev i‡³i bgybv msMÖn Ki‡eb?','8.Are you collecting stool or bloodfrom this person right now?','','q9','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:115" ht="90.75">
       <c r="A10" s="29">
         <v>9</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>47</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>172</v>
+      <c r="E10" s="23" t="s">
+        <v>51</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>173</v>
+        <v>52</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -2234,15 +2256,15 @@
       <c r="U10" s="40"/>
       <c r="V10" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'q7','frmtext', 'tblMainQuesL','7. Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)','7.Enter the name of the individual (check against your ID list from Day1 team)','','q8','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:115" s="40" customFormat="1" ht="75.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'q9','frmsinglechoice', 'tblMainQuesL','9.D³ e¨w³ †_‡K gj/cvqLvbvi bgybv msMÖn Kiv n‡q‡Q wK?','9.Has a stool sample been collected from this individual?','','q10','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:115" ht="90">
       <c r="A11" s="29">
         <v>10</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>47</v>
@@ -2250,15 +2272,24 @@
       <c r="D11" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E11" s="45" t="s">
-        <v>215</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>183</v>
+      <c r="E11" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>50</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
       <c r="R11" s="40" t="s">
         <v>126</v>
       </c>
@@ -2268,42 +2299,34 @@
       <c r="T11" s="40" t="s">
         <v>127</v>
       </c>
+      <c r="U11" s="40"/>
       <c r="V11" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('10', 'q8','frmsinglechoice', 'tblMainQuesL','8.Avcwb wK GLb D³ e¨w³ †_‡K cvqLvbv ev i‡³i bgybv msMÖn Ki‡eb?','8.Are you collecting stool or bloodfrom this person right now?','','q9','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:115" ht="75.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('10', 'q10','frmsinglechoice', 'tblMainQuesL','10.‡Kb cvqLvbvi bgybv msMÖn Kiv hvqwb?','10.Why has a stool sample not been collected?  ','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:115" s="40" customFormat="1" ht="90.75">
       <c r="A12" s="29">
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>47</v>
+        <v>213</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="23" t="s">
-        <v>51</v>
+      <c r="E12" s="37" t="s">
+        <v>214</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>52</v>
+        <v>215</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
+        <v>160</v>
+      </c>
       <c r="R12" s="40" t="s">
         <v>126</v>
       </c>
@@ -2313,43 +2336,33 @@
       <c r="T12" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="U12" s="40"/>
       <c r="V12" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('11', 'q9','frmsinglechoice', 'tblMainQuesL','9.D³ e¨w³ †_‡K gj/cvqLvbvi bgybv msMÖn Kiv n‡q‡Q wK?','9.Has a stool sample been collected from this individual?','','q10','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:115" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('11', 'q10_other','frmtext', 'tblMainQuesL','10.Ab¨vY¨t wbw`©ó K‡i wjLyb','10.Other: Specify','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:115" s="40" customFormat="1" ht="105">
       <c r="A13" s="29">
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>55</v>
+        <v>27</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>223</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
+        <v>160</v>
+      </c>
       <c r="R13" s="40" t="s">
         <v>126</v>
       </c>
@@ -2359,34 +2372,42 @@
       <c r="T13" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="U13" s="40"/>
       <c r="V13" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('12', 'q10','frmsinglechoice', 'tblMainQuesL','10.‡Kb cvqLvbvi bgybv msMÖn Kiv hvqwb?','10.Why has a stool sample not been collected?  ','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:115" s="40" customFormat="1" ht="75.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('12', 'msg01','frmmessage', 'tblMainQues','D³ LvbvwU bZzb BB wm‡½j Av‡g©i AšÍ©fz³ wn‡m‡e wb‡`©k Ki‡Z ev †evSv‡Z msMÖnK…Z ÷zj K‡›UBbv‡ii wQwci Dci ZviKv wPý (*) emvb','NOTE: Mark the cap of the stool collection containersin this household with * to show that this household is in the single arm EE cohort.','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:115" ht="157.5">
       <c r="A14" s="29">
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>216</v>
+        <v>160</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>49</v>
+        <v>156</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E14" s="37" t="s">
-        <v>217</v>
+      <c r="E14" s="27" t="s">
+        <v>181</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>161</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
       <c r="R14" s="40" t="s">
         <v>126</v>
       </c>
@@ -2396,32 +2417,33 @@
       <c r="T14" s="40" t="s">
         <v>127</v>
       </c>
+      <c r="U14" s="40"/>
       <c r="V14" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('13', 'q10_other','frmtext', 'tblMainQuesL','10.Ab¨vY¨t wbw`©ó K‡i wjLyb','10.Other: Specify','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:115" ht="157.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('13', 'msg02','frmmessage', 'tblMainQuesL','wbwðZ Kiæb †h cvqLvbvi bgybv cixÿv Kivi Rb¨ Avcwb K¨v‡Uv-K¨vUR GwjKU ˆZix K‡i‡Qb Ges K¨v‡Uv-K¨vUR GwjK‡Ui Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q| ','Make sure that you have prepared a Kato-Katz aliquot for this individual and make sure that the sample ID and random ID of the barcode on the Kato-Katz aliquot match the following:','','q11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:115" ht="90">
       <c r="A15" s="29">
         <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>156</v>
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>143</v>
       </c>
       <c r="E15" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>185</v>
-      </c>
       <c r="H15" s="29" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -2444,30 +2466,30 @@
       <c r="U15" s="40"/>
       <c r="V15" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('14', 'msg02','frmmessage', 'tblMainQuesL','wbwðZ Kiæb †h cvqLvbvi bgybv cixÿv Kivi Rb¨ Avcwb K¨v‡Uv-K¨vUR GwjKU ˆZix K‡i‡Qb Ges K¨v‡Uv-K¨vUR GwjK‡Ui Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q| ','Make sure that you have prepared a Kato-Katz aliquot for this individual and make sure that the sample ID and random ID of the barcode on the Kato-Katz aliquot match the following:','','q11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:115" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('14', 'q11','frmyeartomin', 'tblMainQuesL','11.msM„nxZ bgybv Kyje†· ivLvi ïiæi mgqUv wjwce× Kiæb (24 N›Uv wnmv‡e)','11.Enter the cold chain start time  (24-hr scale)','','q12','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:115" ht="90">
       <c r="A16" s="29">
         <v>15</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>47</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>143</v>
       </c>
       <c r="E16" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="F16" s="26" t="s">
-        <v>187</v>
-      </c>
       <c r="H16" s="29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -2490,15 +2512,15 @@
       <c r="U16" s="40"/>
       <c r="V16" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('15', 'q11','frmyeartomin', 'tblMainQuesL','11.msM„nxZ bgybv Kyje†· ivLvi ïiæi mgqUv wjwce× Kiæb (24 N›Uv wnmv‡e)','11.Enter the cold chain start time  (24-hr scale)','','q12','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('15', 'q12','frmsinglechoice', 'tblMainQuesL','12.(পর্যবেক্ষন করুন) cvqLvbvi aib †Kgb?','12.(obs) Stool consistency','','q13','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="90">
       <c r="A17" s="29">
         <v>16</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>47</v>
@@ -2507,13 +2529,13 @@
         <v>143</v>
       </c>
       <c r="E17" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>189</v>
-      </c>
       <c r="H17" s="29" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -2536,27 +2558,27 @@
       <c r="U17" s="40"/>
       <c r="V17" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('16', 'q12','frmsinglechoice', 'tblMainQuesL','12.(পর্যবেক্ষন করুন) cvqLvbvi aib †Kgb?','12.(obs) Stool consistency','','q13','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('16', 'q13','frmsinglechoice', 'tblMainQuesL','13.(পর্যবেক্ষন করুন) cvqLvbvi eb© wK?','13. (obs) Stool color','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="90.75">
       <c r="A18" s="29">
         <v>17</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>47</v>
+        <v>161</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>191</v>
       </c>
       <c r="H18" s="29" t="s">
         <v>73</v>
@@ -2582,30 +2604,30 @@
       <c r="U18" s="40"/>
       <c r="V18" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('17', 'q13','frmsinglechoice', 'tblMainQuesL','13.(পর্যবেক্ষন করুন) cvqLvbvi eb© wK?','13. (obs) Stool color','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="75.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('17', 'q13_other','frmtext', 'tblMainQuesL','13.Ab¨vY¨t wbw`©ó K‡i wjLyb','13.Other: Specify','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="90">
       <c r="A19" s="29">
         <v>18</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>49</v>
+        <v>73</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>35</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F19" s="26" t="s">
-        <v>193</v>
-      </c>
       <c r="H19" s="29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -2628,28 +2650,29 @@
       <c r="U19" s="40"/>
       <c r="V19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('18', 'q13_other','frmtext', 'tblMainQuesL','13.Ab¨vY¨t wbw`©ó K‡i wjLyb','13.Other: Specify','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('18', 'q14','frmmultiplechoice', 'tblMainQuesL','14. (পর্যবেক্ষন করুন) msM„nxZ cvqLvbvi bgybvi g‡a¨ A¯^vfvweK wKQz †`Lv †M‡Q wK? (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','14.(obs) Do you see any abnormal characteristics of the collected stool sample? (Select all that apply)','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="90.75">
       <c r="A20" s="29">
         <v>19</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>47</v>
+        <v>162</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="F20" s="26" t="s">
-        <v>195</v>
-      </c>
+      <c r="G20" s="36"/>
       <c r="H20" s="29" t="s">
         <v>74</v>
       </c>
@@ -2674,31 +2697,30 @@
       <c r="U20" s="40"/>
       <c r="V20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('19', 'q14','frmsinglechoice', 'tblMainQuesL','14. (পর্যবেক্ষন করুন) msM„nxZ cvqLvbvi bgybvi g‡a¨ A¯^vfvweK wKQz †`Lv †M‡Q wK? (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','14.(obs) Do you see any abnormal characteristics of the collected stool sample? (Select all that apply)','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="75.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('19', 'q14_other','frmtext', 'tblMainQuesL','14.Ab¨vY¨t wbw`©ó K‡i wjLyb','14.Other: Specify','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="90">
       <c r="A21" s="29">
         <v>20</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>49</v>
+        <v>74</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>47</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E21" s="37" t="s">
-        <v>196</v>
+      <c r="E21" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="G21" s="36"/>
+        <v>195</v>
+      </c>
       <c r="H21" s="29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
@@ -2721,30 +2743,30 @@
       <c r="U21" s="40"/>
       <c r="V21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('20', 'q14_other','frmtext', 'tblMainQuesL','14.Ab¨vY¨t wbw`©ó K‡i wjLyb','14.Other: Specify','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('20', 'q15','frmsinglechoice', 'tblMainQuesL','15.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','15.Enter the day of defecation','','q16','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="90">
       <c r="A22" s="29">
         <v>21</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>47</v>
+        <v>76</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>67</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>143</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>197</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -2767,27 +2789,27 @@
       <c r="U22" s="40"/>
       <c r="V22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('21', 'q15','frmsinglechoice', 'tblMainQuesL','15.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','15.Enter the day of defecation','','q16','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('21', 'q16','frmyeartomin', 'tblMainQuesL','16.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi mgq wjwce× Kiæb (24 N›Uv wnmv‡e, Rvwb bv n‡j 99:99 emvb)','16.Enter the time of defecation (24-hr scale, enter 99:99 for DK)','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="90">
       <c r="A23" s="29">
         <v>22</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>67</v>
+        <v>93</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>47</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>143</v>
       </c>
       <c r="E23" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23" s="26" t="s">
         <v>199</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>200</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>94</v>
@@ -2813,15 +2835,15 @@
       <c r="U23" s="40"/>
       <c r="V23" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('22', 'q16','frmyeartomin', 'tblMainQuesL','16.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi mgq wjwce× Kiæb (24 N›Uv wnmv‡e, Rvwb bv n‡j 99:99 emvb)','16.Enter the time of defecation (24-hr scale, enter 99:99 for DK)','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('22', 'q17','frmsinglechoice', 'tblMainQuesL','17.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','17.Enter the approximate time of defecation','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" s="40" customFormat="1" ht="90">
       <c r="A24" s="29">
         <v>23</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>47</v>
@@ -2829,24 +2851,15 @@
       <c r="D24" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="F24" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="F24" s="26" t="s">
-        <v>202</v>
-      </c>
       <c r="H24" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24"/>
-      <c r="P24"/>
-      <c r="Q24"/>
+        <v>167</v>
+      </c>
       <c r="R24" s="40" t="s">
         <v>126</v>
       </c>
@@ -2856,18 +2869,17 @@
       <c r="T24" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="U24" s="40"/>
       <c r="V24" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('23', 'q17','frmsinglechoice', 'tblMainQuesL','17.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','17.Enter the approximate time of defecation','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" s="40" customFormat="1" ht="82.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('23', 'q18','frmsinglechoice', 'tblMainQuesL','18.cvqLvbvi bgybvwU GKev‡I Kiv cvqLvbv †_‡K bvwKGKvwaKevi Kiv cvqLvbv †_‡K msMÖn Kiv n‡q‡Q?','18.Was the stool collected from one defecation event or multiple defecation events?','','q19a','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="90">
       <c r="A25" s="29">
         <v>24</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>94</v>
+        <v>167</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>47</v>
@@ -2875,15 +2887,24 @@
       <c r="D25" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" s="26" t="s">
         <v>203</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>204</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>168</v>
       </c>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
       <c r="R25" s="40" t="s">
         <v>126</v>
       </c>
@@ -2893,12 +2914,13 @@
       <c r="T25" s="40" t="s">
         <v>127</v>
       </c>
+      <c r="U25" s="40"/>
       <c r="V25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('24', 'q18','frmsinglechoice', 'tblMainQuesL','18.cvqLvbvi bgybvwU GKev‡I Kiv cvqLvbv †_‡K bvwKGKvwaKevi Kiv cvqLvbv †_‡K msMÖn Kiv n‡q‡Q?','18.Was the stool collected from one defecation event or multiple defecation events?','','q19a','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('24', 'q19a','frmsinglechoice', 'tblMainQuesL','19.K.(পর্যবেক্ষন করুন) D³ e¨w³/wkï cv‡q RyZv c‡o‡Q wK ?','19.a. (obs) Is the individual wearing shoes? ','','q19b','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="40" customFormat="1" ht="90">
       <c r="A26" s="29">
         <v>25</v>
       </c>
@@ -2911,24 +2933,15 @@
       <c r="D26" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="F26" s="47" t="s">
         <v>205</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>206</v>
-      </c>
       <c r="H26" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-      <c r="P26"/>
-      <c r="Q26"/>
+        <v>163</v>
+      </c>
       <c r="R26" s="40" t="s">
         <v>126</v>
       </c>
@@ -2938,33 +2951,32 @@
       <c r="T26" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="U26" s="40"/>
       <c r="V26" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('25', 'q19a','frmsinglechoice', 'tblMainQuesL','19.K.(পর্যবেক্ষন করুন) D³ e¨w³/wkï cv‡q RyZv c‡o‡Q wK ?','19.a. (obs) Is the individual wearing shoes? ','','q19b','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" s="40" customFormat="1" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('25', 'q19b','frmsinglechoice', 'tblMainQuesL','19.L.BB wUg D³ Uv‡M©U wkï (Ges Uv‡M©U wkïi RgR) †_‡K i‡³i bgybv msMÖn K‡i‡Q wK ? ','19.b. Has a target child (and twin) blood sample already been collected by the EE team? ','','msg03','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" s="40" customFormat="1" ht="90">
       <c r="A27" s="29">
         <v>26</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E27" s="46" t="s">
-        <v>207</v>
-      </c>
-      <c r="F27" s="47" t="s">
-        <v>208</v>
+      <c r="E27" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>165</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>164</v>
+        <v>65</v>
       </c>
       <c r="R27" s="40" t="s">
         <v>126</v>
@@ -2977,31 +2989,40 @@
       </c>
       <c r="V27" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('26', 'q19b','frmsinglechoice', 'tblMainQuesL','19.L.BB wUg D³ Uv‡M©U wkï (Ges Uv‡M©U wkïi RgR) †_‡K i‡³i bgybv msMÖn K‡i‡Q wK ? ','19.b. Has a target child (and twin) blood sample already been collected by the EE team? ','','msg03','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" s="40" customFormat="1" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('26', 'msg03','frmmessage', 'tblMainQuesL','D³ Lvbvi Uv‡M©U wkï Ges Uv‡M©U wkïi RgR †_‡K i‡³i bgybv msMÖn Ki‡Z n‡ebv|','Do not collect a blood sample from target child (and twin) in this household','','q20','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="90">
       <c r="A28" s="29">
         <v>27</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>164</v>
+        <v>65</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>156</v>
+        <v>47</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E28" s="31" t="s">
-        <v>165</v>
+      <c r="E28" s="27" t="s">
+        <v>118</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>65</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
       <c r="R28" s="40" t="s">
         <v>126</v>
       </c>
@@ -3011,9 +3032,10 @@
       <c r="T28" s="40" t="s">
         <v>127</v>
       </c>
+      <c r="U28" s="40"/>
       <c r="V28" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('27', 'msg03','frmmessage', 'tblMainQuesL','D³ Lvbvi Uv‡M©U wkï Ges Uv‡M©U wkïi RgR †_‡K i‡³i bgybv msMÖn Ki‡Z n‡ebv|','Do not collect a blood sample from target child (and twin) in this household','','q20','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('27', 'q20','frmsinglechoice', 'tblMainQuesL','20.D³ e¨w³/ wkï †_‡K i‡³i bgybv msMÖn Kiv n‡q‡Q wK?','20.Has a blood sample been collected from this individual?','','q21','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="90">
@@ -3021,7 +3043,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>47</v>
@@ -3030,13 +3052,13 @@
         <v>143</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F29" s="26" t="s">
-        <v>226</v>
+        <v>121</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I29"/>
       <c r="J29"/>
@@ -3059,40 +3081,31 @@
       <c r="U29" s="40"/>
       <c r="V29" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('28', 'q20','frmsinglechoice', 'tblMainQuesL','20.D³ e¨w³/ wkï †_‡K i‡³i bgybv msMÖn Kiv n‡q‡Q wK?','20.Has a blood sample been collected from this individual?','','q21','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('28', 'q21','frmsinglechoice', 'tblMainQuesL','21.‡Kb i‡³i bgybv msMÖn Kiv hvqwb?','21.Why has a blood sample not been collected?','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" s="40" customFormat="1" ht="90.75">
       <c r="A30" s="29">
         <v>29</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>47</v>
+        <v>179</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E30" s="27" t="s">
-        <v>120</v>
+      <c r="E30" s="37" t="s">
+        <v>206</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>121</v>
+        <v>207</v>
       </c>
       <c r="H30" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-      <c r="N30"/>
-      <c r="O30"/>
-      <c r="P30"/>
-      <c r="Q30"/>
       <c r="R30" s="40" t="s">
         <v>126</v>
       </c>
@@ -3102,34 +3115,42 @@
       <c r="T30" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="U30" s="40"/>
       <c r="V30" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('29', 'q21','frmsinglechoice', 'tblMainQuesL','21.‡Kb i‡³i bgybv msMÖn Kiv hvqwb?','21.Why has a blood sample not been collected?','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" s="40" customFormat="1" ht="75.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('29', 'q21_other','frmtext', 'tblMainQuesL','21.Ab¨vY¨t wbw`©ó K‡i wjLyb','21.Other: Specify','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="90">
       <c r="A31" s="29">
         <v>30</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>182</v>
+        <v>119</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="F31" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="F31" s="26" t="s">
-        <v>210</v>
-      </c>
       <c r="H31" s="29" t="s">
-        <v>119</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
       <c r="R31" s="40" t="s">
         <v>126</v>
       </c>
@@ -3139,32 +3160,33 @@
       <c r="T31" s="40" t="s">
         <v>127</v>
       </c>
+      <c r="U31" s="40"/>
       <c r="V31" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('30', 'q21_other','frmtext', 'tblMainQuesL','21.Ab¨vY¨t wbw`©ó K‡i wjLyb','21.Other: Specify','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('30', 'q22','frmnumeric', 'tblMainQuesL','22. A¨vwbwgqv †U‡÷i djvdj wjLyb ','22.Enter the result of the anemia test. __ __. __ g/dL','','msg04','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="115.5">
       <c r="A32" s="29">
         <v>31</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="F32" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="F32" s="26" t="s">
-        <v>212</v>
-      </c>
       <c r="H32" s="29" t="s">
-        <v>167</v>
+        <v>122</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -3187,31 +3209,29 @@
       <c r="U32" s="40"/>
       <c r="V32" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('31', 'q22','frmnumeric', 'tblMainQuesL','22. A¨vwbwgqv †U‡÷i djvdj wjLyb ','22.Enter the result of the anemia test. __ __. __ g/dL','','msg04','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" ht="120">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('31', 'msg04','frmmessage', 'tblMainQuesL','wbwðZ Kiæb eøvW ¯úU wdëvi †ccv‡ii Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q|','Make sure that the sample ID and random ID of the barcode on the blood spot filter paper match the following:','','q23','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="90">
       <c r="A33" s="29">
         <v>32</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>167</v>
+        <v>122</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="31" t="s">
-        <v>213</v>
+      <c r="E33" s="27" t="s">
+        <v>123</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>122</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="H33" s="29"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -3233,52 +3253,26 @@
       <c r="U33" s="40"/>
       <c r="V33" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('32', 'msg04','frmmessage', 'tblMainQuesL','wbwðZ Kiæb eøvW ¯úU wdëvi †ccv‡ii Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q|','Make sure that the sample ID and random ID of the barcode on the blood spot filter paper match the following:','','q23','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" ht="78.75">
-      <c r="A34" s="29">
-        <v>33</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E34" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="H34" s="29"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="S34" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T34" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="U34" s="40"/>
-      <c r="V34" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('33', 'q23','frmnumeric', 'tblMainQuesL','23.wdëvi †ccv‡i i‡³i Kq‡dvUv bgybv msMÖn Kiv n‡q‡Q Zvi msL¨v wjLyb (msL¨v 1 †_‡K 6 Gi g‡a¨ n‡e)','23.Enter the number of spots filled (has to be between 1 and 6)','','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('32', 'q23','frmnumeric', 'tblMainQuesL','23.wdëvi †ccv‡i i‡³i Kq‡dvUv bgybv msMÖn Kiv n‡q‡Q Zvi msL¨v wjLyb (msL¨v 1 †_‡K 6 Gi g‡a¨ n‡e)','23.Enter the number of spots filled (has to be between 1 and 6)','','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="E45" s="25"/>
+      <c r="H45" s="29"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
     </row>
     <row r="46" spans="1:22">
       <c r="A46" s="29"/>
@@ -10373,25 +10367,7 @@
       <c r="T439"/>
     </row>
     <row r="440" spans="1:20">
-      <c r="A440" s="29"/>
-      <c r="B440" s="29"/>
       <c r="E440" s="25"/>
-      <c r="H440" s="29"/>
-      <c r="I440"/>
-      <c r="J440"/>
-      <c r="K440"/>
-      <c r="L440"/>
-      <c r="M440"/>
-      <c r="N440"/>
-      <c r="O440"/>
-      <c r="P440"/>
-      <c r="Q440"/>
-      <c r="R440"/>
-      <c r="S440"/>
-      <c r="T440"/>
-    </row>
-    <row r="441" spans="1:20">
-      <c r="E441" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10401,10 +10377,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1261"/>
+  <dimension ref="A1:G1263"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G58"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -10446,7 +10422,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>45</v>
@@ -10459,7 +10435,7 @@
       </c>
       <c r="G2" s="22" t="str">
         <f>"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A2&amp;"','" &amp;B2&amp;"', '" &amp;D2&amp;"','" &amp;C2&amp;"','" &amp;E2&amp;"','"&amp;F2&amp;"');"</f>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('1','qspilid', '1.Yes ','1.n¨v','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('1','qSpil', '1.Yes ','1.n¨v','1','');</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
@@ -10467,7 +10443,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>46</v>
@@ -10478,12 +10454,10 @@
       <c r="E3" s="40">
         <v>2</v>
       </c>
-      <c r="F3" s="29" t="s">
-        <v>31</v>
-      </c>
+      <c r="F3" s="29"/>
       <c r="G3" s="22" t="str">
-        <f t="shared" ref="G3:G58" si="0">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;D3&amp;"','" &amp;C3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('2','qspilid', '2.No  ','2.bv','2','q3');</v>
+        <f t="shared" ref="G3:G60" si="0">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;D3&amp;"','" &amp;C3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('2','qSpil', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30">
@@ -10659,7 +10633,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>146</v>
@@ -10680,7 +10654,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>147</v>
@@ -10701,7 +10675,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>148</v>
@@ -10722,7 +10696,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>145</v>
@@ -10743,7 +10717,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16" s="29" t="s">
         <v>144</v>
@@ -10764,7 +10738,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>152</v>
@@ -10788,10 +10762,10 @@
         <v>48</v>
       </c>
       <c r="C18" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="40" t="s">
         <v>174</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>175</v>
       </c>
       <c r="E18" s="42">
         <v>1</v>
@@ -10801,49 +10775,46 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('17','q8', '1.Stool','1.cvqLvbv','1','');</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="40" customFormat="1" ht="30">
+    <row r="19" spans="1:7" s="40" customFormat="1" ht="30.75">
       <c r="A19" s="40">
         <v>18</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="41" t="s">
-        <v>176</v>
+      <c r="C19" s="37" t="s">
+        <v>221</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="E19" s="42">
         <v>2</v>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('18','q8', '2.Blood','2.i‡³i bgybv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('18','q8', '2.Stool and blood','2.cvqLvbv + i‡³i bgybv','2','');</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="40" customFormat="1" ht="30">
       <c r="A20" s="40">
         <v>19</v>
       </c>
-      <c r="B20" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="E20" s="34">
-        <v>1</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>161</v>
+      <c r="B20" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="42">
+        <v>3</v>
       </c>
       <c r="G20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('19','q9', '1.Yes ','1.n¨v','1','msg02');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('19','q8', '3.Blood','3.i‡³i bgybv','3','');</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="40" customFormat="1" ht="30">
@@ -10854,18 +10825,20 @@
         <v>50</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E21" s="34">
-        <v>2</v>
-      </c>
-      <c r="F21"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>160</v>
+      </c>
       <c r="G21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('20','q9', '2.No  ','2.bv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('20','q9', '1.Yes ','1.n¨v','1','msg02');</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="40" customFormat="1" ht="30">
@@ -10873,21 +10846,21 @@
         <v>21</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="34"/>
+        <v>50</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="34">
+        <v>2</v>
+      </c>
+      <c r="F22"/>
       <c r="G22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('21','q10', '1.Subject not available','1.D³ e¨w³ Dcw¯’Z wQj bv','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('21','q9', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="40" customFormat="1" ht="30">
@@ -10898,18 +10871,18 @@
         <v>54</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('22','q10', '2.Subject not cooperative','2.D³ e¨w³ mn‡hvwMZv K‡iwb','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('22','q10', '1.Subject not available','1.D³ e¨w³ Dcw¯’Z wQj bv','1','');</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="40" customFormat="1" ht="30">
@@ -10920,18 +10893,18 @@
         <v>54</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('23','q10', '3.Sample not available','3.bgybv cvIqv hvqwb','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('23','q10', '2.Subject not cooperative','2.D³ e¨w³ mn‡hvwMZv K‡iwb','2','');</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="40" customFormat="1" ht="30">
@@ -10941,42 +10914,43 @@
       <c r="B25" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="43" t="s">
-        <v>64</v>
+      <c r="C25" s="41" t="s">
+        <v>61</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>216</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F25" s="34"/>
       <c r="G25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('24','q10', '4.Other','4.Ab¨vb¨','4','q10_other');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('24','q10', '3.Sample not available','3.bgybv cvIqv hvqwb','3','');</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="40" customFormat="1" ht="30">
       <c r="A26" s="40">
         <v>25</v>
       </c>
-      <c r="B26" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>88</v>
+      <c r="B26" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>213</v>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('25','q12', '1.Unformed, watery','1.AmsMwVZ, Zij','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('25','q10', '4.Other','4.Ab¨vb¨','4','q10_other');</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="40" customFormat="1" ht="30">
@@ -10987,17 +10961,17 @@
         <v>66</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('26','q12', '2.Formed, soft, moist','2.msMwVZ, big, ‡fRv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('26','q12', '1.Unformed, watery','1.AmsMwVZ, Zij','1','');</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11008,17 +10982,17 @@
         <v>66</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>90</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('27','q12', '3.Formed, hard, dry','3.msMwVZ, k³, ïKbv','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('27','q12', '2.Formed, soft, moist','2.msMwVZ, big, ‡fRv','2','');</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11026,21 +11000,20 @@
         <v>28</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>97</v>
+        <v>91</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>92</v>
       </c>
       <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29"/>
+        <v>3</v>
+      </c>
       <c r="G29" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('28','q13', '1.Yellow','1.njy`','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('28','q12', '3.Formed, hard, dry','3.msMwVZ, k³, ïKbv','3','');</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11051,18 +11024,18 @@
         <v>68</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30"/>
       <c r="G30" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('29','q13', '2.Brown','2.ev`vgx','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('29','q13', '1.Yellow','1.njy`','1','');</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11073,18 +11046,18 @@
         <v>68</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31"/>
       <c r="G31" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('30','q13', '3.Black','3.Kv‡jv','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('30','q13', '2.Brown','2.ev`vgx','2','');</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11095,18 +11068,18 @@
         <v>68</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32"/>
       <c r="G32" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('31','q13', '4.Green','4.meyR','4','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('31','q13', '3.Black','3.Kv‡jv','3','');</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11117,18 +11090,18 @@
         <v>68</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33"/>
       <c r="G33" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('32','q13', '5.White/grey','5.mv`v/aymi','5','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('32','q13', '4.Green','4.meyR','4','');</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11139,20 +11112,18 @@
         <v>68</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E34">
-        <v>6</v>
-      </c>
-      <c r="F34" s="40" t="s">
-        <v>162</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F34"/>
       <c r="G34" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('33','q13', '6.Other: Specify','6.Ab¨vY¨t wbw`©ó K‡i wjLyb','6','q13_other');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('33','q13', '5.White/grey','5.mv`v/aymi','5','');</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11160,21 +11131,23 @@
         <v>34</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35"/>
+        <v>6</v>
+      </c>
+      <c r="F35" s="40" t="s">
+        <v>161</v>
+      </c>
       <c r="G35" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('34','q14', '1.No abnormal characteristics','1.A¯^vfvweK wKQz †`Lv hvqwb','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('34','q13', '6.Other: Specify','6.Ab¨vY¨t wbw`©ó K‡i wjLyb','6','q13_other');</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11182,21 +11155,21 @@
         <v>35</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>73</v>
+        <v>226</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36"/>
       <c r="G36" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('35','q14', '2.Mucus','2.†kø®§v ev K‡di gZ wcQj g‡b n‡q‡Q','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('35','q14_1', '1.No abnormal characteristics','1.A¯^vfvweK wKQz †`Lv hvqwb','1','');</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11204,21 +11177,21 @@
         <v>36</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>73</v>
+        <v>227</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F37"/>
       <c r="G37" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('36','q14', '3.Blood','3.gj/cvqLvbvi mv‡_ i³ †`Lv †M‡Q','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('36','q14_2', '2.Mucus','2.†kø®§v ev K‡di gZ wcQj g‡b n‡q‡Q','1','');</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11226,21 +11199,21 @@
         <v>37</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>73</v>
+        <v>228</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F38"/>
       <c r="G38" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('37','q14', '4.Worms','4.K„wg †`Lv †M‡Q','4','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('37','q14_3', '3.Blood','3.gj/cvqLvbvi mv‡_ i³ †`Lv †M‡Q','1','');</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11248,23 +11221,21 @@
         <v>38</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>73</v>
+        <v>229</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E39">
-        <v>5</v>
-      </c>
-      <c r="F39" s="40" t="s">
-        <v>163</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F39"/>
       <c r="G39" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('38','q14', '5.Other: Specify','5.Ab¨vY¨t wbw`©ó K‡i wjLyb','5','q14_other');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('38','q14_4', '4.Worms','4.K„wg †`Lv †M‡Q','1','');</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11272,23 +11243,26 @@
         <v>39</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>74</v>
+        <v>230</v>
       </c>
       <c r="C40" s="41" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
+      <c r="F40" s="40" t="s">
+        <v>162</v>
+      </c>
       <c r="G40" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('39','q15', '1.Today','1.AvR','1','');</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('39','q14_5', '5.Other: Specify','5.Ab¨vY¨t wbw`©ó K‡i wjLyb','1','q14_other');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="40" customFormat="1" ht="30">
       <c r="A41" s="40">
         <v>40</v>
       </c>
@@ -11296,17 +11270,17 @@
         <v>74</v>
       </c>
       <c r="C41" s="41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('40','q15', '2.Yesterday','2.MZKvj','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('40','q15', '1.Today','1.AvR','1','');</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30">
@@ -11314,20 +11288,20 @@
         <v>41</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C42" s="41" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('41','q17', '1.Morning','1.mKvj','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('41','q15', '2.Yesterday','2.MZKvj','2','');</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30">
@@ -11338,17 +11312,17 @@
         <v>93</v>
       </c>
       <c r="C43" s="41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('42','q17', '2.Noon','2.`ycyi','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('42','q17', '1.Morning','1.mKvj','1','');</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30">
@@ -11359,17 +11333,17 @@
         <v>93</v>
       </c>
       <c r="C44" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G44" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('43','q17', '3.Afternoon','3.weKvj','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('43','q17', '2.Noon','2.`ycyi','2','');</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30">
@@ -11380,17 +11354,17 @@
         <v>93</v>
       </c>
       <c r="C45" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G45" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('44','q17', '4.Evening','4.mÜ¨v','4','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('44','q17', '3.Afternoon','3.weKvj','3','');</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30">
@@ -11401,38 +11375,38 @@
         <v>93</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G46" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('45','q17', '5.Night','5.ivZ','5','');</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" s="40" customFormat="1" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('45','q17', '4.Evening','4.mÜ¨v','4','');</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30">
       <c r="A47" s="40">
         <v>46</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="41" t="s">
-        <v>178</v>
+        <v>85</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="E47" s="40">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
       </c>
       <c r="G47" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('46','q18', '1.Single','1.GKev‡I Kiv cvqLvbv †_‡K','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('46','q17', '5.Night','5.ivZ','5','');</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="40" customFormat="1" ht="30">
@@ -11443,38 +11417,38 @@
         <v>94</v>
       </c>
       <c r="C48" s="41" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E48" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('47','q18', '2.Multiple','2.GKvwaKev‡I Kiv cvqLvbv †_‡K','2','');</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('47','q18', '1.Single','1.GKev‡I Kiv cvqLvbv †_‡K','1','');</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="40" customFormat="1" ht="30">
       <c r="A49" s="40">
         <v>48</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49" s="44" t="s">
-        <v>45</v>
+        <v>94</v>
+      </c>
+      <c r="C49" s="41" t="s">
+        <v>177</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="E49" s="34">
-        <v>1</v>
+        <v>178</v>
+      </c>
+      <c r="E49" s="40">
+        <v>2</v>
       </c>
       <c r="G49" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('48','q19a', '1.Yes ','1.n¨v','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('48','q18', '2.Multiple','2.GKvwaKev‡I Kiv cvqLvbv †_‡K','2','');</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30">
@@ -11482,20 +11456,20 @@
         <v>49</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G50" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('49','q19a', '2.No  ','2.bv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('49','q19a', '1.Yes ','1.n¨v','1','');</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30">
@@ -11503,49 +11477,49 @@
         <v>50</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="E51" s="34">
+        <v>2</v>
       </c>
       <c r="G51" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('50','q19b', '1.Yes ','1.n¨v','1','');</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('50','q19a', '2.No  ','2.bv','2','');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="40" customFormat="1" ht="30">
       <c r="A52" s="40">
         <v>51</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>46</v>
+        <v>224</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="E52">
-        <v>2</v>
+        <v>225</v>
+      </c>
+      <c r="E52" s="40">
+        <v>3</v>
       </c>
       <c r="G52" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('51','q19b', '2.No  ','2.bv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('51','q19a', '3.Could not observe','3.ch©‡eÿb Kiv m¤¢e nqwb','3','');</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30">
       <c r="A53" s="40">
         <v>52</v>
       </c>
-      <c r="B53" s="36" t="s">
-        <v>65</v>
+      <c r="B53" s="29" t="s">
+        <v>168</v>
       </c>
       <c r="C53" s="44" t="s">
         <v>45</v>
@@ -11553,20 +11527,20 @@
       <c r="D53" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="E53" s="36">
+      <c r="E53">
         <v>1</v>
       </c>
       <c r="G53" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('52','q20', '1.Yes ','1.n¨v','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('52','q19b', '1.Yes ','1.n¨v','1','');</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30">
       <c r="A54" s="40">
         <v>53</v>
       </c>
-      <c r="B54" s="36" t="s">
-        <v>65</v>
+      <c r="B54" s="29" t="s">
+        <v>168</v>
       </c>
       <c r="C54" s="44" t="s">
         <v>46</v>
@@ -11574,12 +11548,12 @@
       <c r="D54" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="E54" s="36">
+      <c r="E54">
         <v>2</v>
       </c>
       <c r="G54" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('53','q20', '2.No  ','2.bv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('53','q19b', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30">
@@ -11587,20 +11561,20 @@
         <v>54</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="C55" s="41" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="C55" s="44" t="s">
+        <v>45</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="E55" s="36">
         <v>1</v>
       </c>
       <c r="G55" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('54','q21', '1.Subject not available','1.D³ e¨w³ Dcw¯’Z wQj bv','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('54','q20', '1.Yes ','1.n¨v','1','');</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30">
@@ -11608,20 +11582,20 @@
         <v>55</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="C56" s="41" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="C56" s="44" t="s">
+        <v>46</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>60</v>
+        <v>154</v>
       </c>
       <c r="E56" s="36">
         <v>2</v>
       </c>
       <c r="G56" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('55','q21', '2.Subject not cooperative','2.D³ e¨w³ mn‡hvwMZv K‡iwb','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('55','q20', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30">
@@ -11632,17 +11606,17 @@
         <v>117</v>
       </c>
       <c r="C57" s="41" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D57" s="38" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E57" s="36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G57" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('56','q21', '3.Sample not available','3.bgybv cvIqv hvqwb','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('56','q21', '1.Subject not available','1.D³ e¨w³ Dcw¯’Z wQj bv','1','');</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30">
@@ -11652,34 +11626,64 @@
       <c r="B58" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="43" t="s">
-        <v>64</v>
+      <c r="C58" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E58" s="36">
-        <v>4</v>
-      </c>
-      <c r="F58" s="29" t="s">
-        <v>182</v>
+        <v>2</v>
       </c>
       <c r="G58" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('57','q21', '4.Other','4.Ab¨vb¨','4','q21_other');</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="C59" s="41"/>
-      <c r="D59"/>
-      <c r="E59"/>
-      <c r="G59"/>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="C60" s="41"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="G60"/>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('57','q21', '2.Subject not cooperative','2.D³ e¨w³ mn‡hvwMZv K‡iwb','2','');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="30">
+      <c r="A59" s="40">
+        <v>58</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E59" s="36">
+        <v>3</v>
+      </c>
+      <c r="G59" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('58','q21', '3.Sample not available','3.bgybv cvIqv hvqwb','3','');</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="30">
+      <c r="A60" s="40">
+        <v>59</v>
+      </c>
+      <c r="B60" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="36">
+        <v>4</v>
+      </c>
+      <c r="F60" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="G60" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('59','q21', '4.Other','4.Ab¨vb¨','4','q21_other');</v>
+      </c>
     </row>
     <row r="61" spans="1:7">
       <c r="C61" s="41"/>
@@ -18886,6 +18890,18 @@
       <c r="D1261"/>
       <c r="E1261"/>
       <c r="G1261"/>
+    </row>
+    <row r="1262" spans="3:7">
+      <c r="C1262" s="41"/>
+      <c r="D1262"/>
+      <c r="E1262"/>
+      <c r="G1262"/>
+    </row>
+    <row r="1263" spans="3:7">
+      <c r="C1263" s="41"/>
+      <c r="D1263"/>
+      <c r="E1263"/>
+      <c r="G1263"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update on 23 April 2015
</commit_message>
<xml_diff>
--- a/SpecimenCollectionForm/DB and Documents/Specimen Collection- Endline Parasite.xlsx
+++ b/SpecimenCollectionForm/DB and Documents/Specimen Collection- Endline Parasite.xlsx
@@ -141,9 +141,6 @@
     <t xml:space="preserve">4.bgybv msMÖ‡ni ZvwiL </t>
   </si>
   <si>
-    <t xml:space="preserve">4. Data of sample collection </t>
-  </si>
-  <si>
     <t>5.†h wkï †_‡K bgybv msMÖ‡ni Rb¨ cÖ_g w`b ÷zj K‡›UBbvi †`Iqv n‡q‡Q Zvi AvBwW wbev©Pb Kiæb (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)</t>
   </si>
   <si>
@@ -788,6 +785,9 @@
   </si>
   <si>
     <t>q14_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Date of sample collection </t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DK440"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="V2" sqref="V2:V33"/>
     </sheetView>
   </sheetViews>
@@ -1871,31 +1871,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>26</v>
       </c>
       <c r="R2" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S2" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T2" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S2" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T2" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="V2" s="22" t="str">
         <f>"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A2&amp;"', '" &amp;B2&amp;"','" &amp;C2&amp;"', '" &amp;D2&amp;"','" &amp;E2&amp;"','" &amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"', '"&amp;K2&amp;"','"&amp;L2&amp;"','"&amp;M2&amp;"','"&amp;N2&amp;"','"&amp;O2&amp;"','"&amp;P2&amp;"','"&amp;Q2&amp;"',"&amp;R2&amp;","&amp;S2&amp;",'"&amp;T2&amp;"');"</f>
@@ -1934,13 +1934,13 @@
       <c r="P3"/>
       <c r="Q3"/>
       <c r="R3" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="S3" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="T3" s="39" t="s">
         <v>126</v>
-      </c>
-      <c r="S3" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="T3" s="39" t="s">
-        <v>127</v>
       </c>
       <c r="V3" s="22" t="str">
         <f t="shared" ref="V3:V33" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
@@ -1961,7 +1961,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" s="26" t="s">
         <v>38</v>
@@ -1979,13 +1979,13 @@
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S4" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T4" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S4" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T4" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U4" s="40"/>
       <c r="V4" s="22" t="str">
@@ -2010,7 +2010,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>40</v>
+        <v>230</v>
       </c>
       <c r="H5" s="29" t="s">
         <v>34</v>
@@ -2025,18 +2025,18 @@
       <c r="P5"/>
       <c r="Q5"/>
       <c r="R5" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S5" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T5" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S5" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T5" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U5" s="40"/>
       <c r="V5" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'q4','frmdate', 'tblMainQues','4.bgybv msMÖ‡ni ZvwiL ','4. Data of sample collection ','','q5','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'q4','frmdate', 'tblMainQues','4.bgybv msMÖ‡ni ZvwiL ','4. Date of sample collection ','','q5','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="6" spans="1:115" ht="94.5">
@@ -2053,13 +2053,13 @@
         <v>27</v>
       </c>
       <c r="E6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>42</v>
-      </c>
       <c r="H6" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -2071,13 +2071,13 @@
       <c r="P6"/>
       <c r="Q6"/>
       <c r="R6" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S6" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T6" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S6" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T6" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U6" s="40"/>
       <c r="V6" s="22" t="str">
@@ -2090,7 +2090,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>30</v>
@@ -2099,13 +2099,13 @@
         <v>27</v>
       </c>
       <c r="E7" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>170</v>
-      </c>
       <c r="H7" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -2117,13 +2117,13 @@
       <c r="P7"/>
       <c r="Q7"/>
       <c r="R7" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S7" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T7" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S7" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T7" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U7" s="40"/>
       <c r="V7" s="22" t="str">
@@ -2136,22 +2136,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>172</v>
-      </c>
       <c r="H8" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -2163,13 +2163,13 @@
       <c r="P8"/>
       <c r="Q8"/>
       <c r="R8" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S8" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T8" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S8" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T8" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U8" s="40"/>
       <c r="V8" s="22" t="str">
@@ -2182,31 +2182,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R9" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S9" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T9" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S9" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T9" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="V9" s="22" t="str">
         <f t="shared" si="0"/>
@@ -2218,22 +2218,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="23" t="s">
+      <c r="F10" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="H10" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -2245,13 +2245,13 @@
       <c r="P10"/>
       <c r="Q10"/>
       <c r="R10" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S10" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T10" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S10" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T10" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U10" s="40"/>
       <c r="V10" s="22" t="str">
@@ -2264,22 +2264,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="27" t="s">
+      <c r="F11" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>56</v>
-      </c>
       <c r="H11" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -2291,13 +2291,13 @@
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S11" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T11" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S11" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T11" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U11" s="40"/>
       <c r="V11" s="22" t="str">
@@ -2310,31 +2310,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E12" s="37" t="s">
+      <c r="F12" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="F12" s="26" t="s">
-        <v>215</v>
-      </c>
       <c r="H12" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R12" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S12" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T12" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S12" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T12" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="V12" s="22" t="str">
         <f t="shared" si="0"/>
@@ -2346,31 +2346,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R13" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S13" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T13" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S13" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T13" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="V13" s="22" t="str">
         <f t="shared" si="0"/>
@@ -2382,22 +2382,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="F14" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="F14" s="26" t="s">
-        <v>182</v>
-      </c>
       <c r="H14" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -2409,13 +2409,13 @@
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S14" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T14" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S14" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T14" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U14" s="40"/>
       <c r="V14" s="22" t="str">
@@ -2428,22 +2428,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>184</v>
-      </c>
       <c r="H15" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -2455,13 +2455,13 @@
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S15" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T15" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S15" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T15" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U15" s="40"/>
       <c r="V15" s="22" t="str">
@@ -2474,22 +2474,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E16" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="F16" s="26" t="s">
-        <v>186</v>
-      </c>
       <c r="H16" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -2501,13 +2501,13 @@
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S16" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T16" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S16" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T16" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U16" s="40"/>
       <c r="V16" s="22" t="str">
@@ -2520,22 +2520,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E17" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>188</v>
-      </c>
       <c r="H17" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -2547,13 +2547,13 @@
       <c r="P17"/>
       <c r="Q17"/>
       <c r="R17" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S17" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T17" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S17" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T17" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U17" s="40"/>
       <c r="V17" s="22" t="str">
@@ -2566,22 +2566,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E18" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="F18" s="26" t="s">
-        <v>190</v>
-      </c>
       <c r="H18" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
@@ -2593,13 +2593,13 @@
       <c r="P18"/>
       <c r="Q18"/>
       <c r="R18" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S18" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T18" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S18" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T18" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U18" s="40"/>
       <c r="V18" s="22" t="str">
@@ -2612,22 +2612,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E19" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="F19" s="26" t="s">
-        <v>192</v>
-      </c>
       <c r="H19" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -2639,13 +2639,13 @@
       <c r="P19"/>
       <c r="Q19"/>
       <c r="R19" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S19" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T19" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S19" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T19" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U19" s="40"/>
       <c r="V19" s="22" t="str">
@@ -2658,23 +2658,23 @@
         <v>19</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E20" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>193</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>194</v>
       </c>
       <c r="G20" s="36"/>
       <c r="H20" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -2686,13 +2686,13 @@
       <c r="P20"/>
       <c r="Q20"/>
       <c r="R20" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S20" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T20" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S20" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T20" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U20" s="40"/>
       <c r="V20" s="22" t="str">
@@ -2705,22 +2705,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E21" s="27" t="s">
+      <c r="F21" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H21" s="29" t="s">
         <v>75</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>76</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
@@ -2732,13 +2732,13 @@
       <c r="P21"/>
       <c r="Q21"/>
       <c r="R21" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S21" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T21" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S21" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T21" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U21" s="40"/>
       <c r="V21" s="22" t="str">
@@ -2751,22 +2751,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E22" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="F22" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="F22" s="28" t="s">
-        <v>197</v>
-      </c>
       <c r="H22" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -2778,13 +2778,13 @@
       <c r="P22"/>
       <c r="Q22"/>
       <c r="R22" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S22" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T22" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S22" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T22" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U22" s="40"/>
       <c r="V22" s="22" t="str">
@@ -2797,22 +2797,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="H23" s="29" t="s">
         <v>93</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>94</v>
       </c>
       <c r="I23"/>
       <c r="J23"/>
@@ -2824,13 +2824,13 @@
       <c r="P23"/>
       <c r="Q23"/>
       <c r="R23" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S23" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T23" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S23" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T23" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U23" s="40"/>
       <c r="V23" s="22" t="str">
@@ -2843,31 +2843,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="F24" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>201</v>
-      </c>
       <c r="H24" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R24" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S24" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T24" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S24" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T24" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="V24" s="22" t="str">
         <f t="shared" si="0"/>
@@ -2879,22 +2879,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="H25" s="29" t="s">
         <v>167</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>168</v>
       </c>
       <c r="I25"/>
       <c r="J25"/>
@@ -2906,13 +2906,13 @@
       <c r="P25"/>
       <c r="Q25"/>
       <c r="R25" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S25" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T25" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S25" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T25" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U25" s="40"/>
       <c r="V25" s="22" t="str">
@@ -2925,31 +2925,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E26" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="F26" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="F26" s="47" t="s">
-        <v>205</v>
-      </c>
       <c r="H26" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R26" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S26" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T26" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S26" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T26" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="V26" s="22" t="str">
         <f t="shared" si="0"/>
@@ -2961,31 +2961,31 @@
         <v>26</v>
       </c>
       <c r="B27" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="C27" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" s="31" t="s">
+      <c r="F27" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="F27" s="26" t="s">
-        <v>165</v>
-      </c>
       <c r="H27" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R27" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S27" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T27" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S27" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T27" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="V27" s="22" t="str">
         <f t="shared" si="0"/>
@@ -2997,22 +2997,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I28"/>
       <c r="J28"/>
@@ -3024,13 +3024,13 @@
       <c r="P28"/>
       <c r="Q28"/>
       <c r="R28" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S28" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T28" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S28" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T28" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U28" s="40"/>
       <c r="V28" s="22" t="str">
@@ -3043,22 +3043,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E29" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="F29" s="26" t="s">
-        <v>121</v>
-      </c>
       <c r="H29" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I29"/>
       <c r="J29"/>
@@ -3070,13 +3070,13 @@
       <c r="P29"/>
       <c r="Q29"/>
       <c r="R29" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S29" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T29" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S29" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T29" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U29" s="40"/>
       <c r="V29" s="22" t="str">
@@ -3089,31 +3089,31 @@
         <v>29</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E30" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="F30" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="F30" s="26" t="s">
-        <v>207</v>
-      </c>
       <c r="H30" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R30" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S30" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T30" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S30" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T30" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="V30" s="22" t="str">
         <f t="shared" si="0"/>
@@ -3125,22 +3125,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E31" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="F31" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="F31" s="26" t="s">
-        <v>209</v>
-      </c>
       <c r="H31" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I31"/>
       <c r="J31"/>
@@ -3152,13 +3152,13 @@
       <c r="P31"/>
       <c r="Q31"/>
       <c r="R31" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S31" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T31" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S31" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T31" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U31" s="40"/>
       <c r="V31" s="22" t="str">
@@ -3171,22 +3171,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E32" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="F32" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="F32" s="26" t="s">
-        <v>211</v>
-      </c>
       <c r="H32" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -3198,13 +3198,13 @@
       <c r="P32"/>
       <c r="Q32"/>
       <c r="R32" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S32" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T32" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S32" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T32" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U32" s="40"/>
       <c r="V32" s="22" t="str">
@@ -3217,19 +3217,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E33" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="27" t="s">
+      <c r="F33" s="26" t="s">
         <v>123</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>124</v>
       </c>
       <c r="H33" s="29"/>
       <c r="I33"/>
@@ -3242,13 +3242,13 @@
       <c r="P33"/>
       <c r="Q33"/>
       <c r="R33" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="S33" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="T33" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="S33" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="T33" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="U33" s="40"/>
       <c r="V33" s="22" t="str">
@@ -10379,7 +10379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G60"/>
     </sheetView>
   </sheetViews>
@@ -10422,13 +10422,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E2" s="40">
         <v>1</v>
@@ -10443,13 +10443,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" s="40">
         <v>2</v>
@@ -10465,13 +10465,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -10486,13 +10486,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="40">
         <v>1</v>
@@ -10507,13 +10507,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="40">
         <v>1</v>
@@ -10528,13 +10528,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="42">
         <v>1</v>
@@ -10549,13 +10549,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="40" t="s">
         <v>141</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>142</v>
       </c>
       <c r="E8" s="42">
         <v>1</v>
@@ -10570,13 +10570,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="40" t="s">
         <v>149</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>150</v>
       </c>
       <c r="E9" s="42">
         <v>1</v>
@@ -10591,13 +10591,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>45</v>
-      </c>
       <c r="D10" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E10" s="33">
         <v>1</v>
@@ -10612,13 +10612,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="33">
         <v>2</v>
@@ -10633,13 +10633,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="40">
         <v>1</v>
@@ -10654,13 +10654,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E13" s="40">
         <v>1</v>
@@ -10675,13 +10675,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" s="40">
         <v>1</v>
@@ -10696,13 +10696,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E15" s="42">
         <v>1</v>
@@ -10717,13 +10717,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" s="42">
         <v>1</v>
@@ -10738,13 +10738,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E17" s="42">
         <v>1</v>
@@ -10759,13 +10759,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="40" t="s">
         <v>173</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>174</v>
       </c>
       <c r="E18" s="42">
         <v>1</v>
@@ -10780,13 +10780,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="40" t="s">
         <v>221</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>222</v>
       </c>
       <c r="E19" s="42">
         <v>2</v>
@@ -10801,13 +10801,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="42">
         <v>3</v>
@@ -10822,19 +10822,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E21" s="34">
         <v>1</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G21" s="22" t="str">
         <f t="shared" si="0"/>
@@ -10846,13 +10846,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E22" s="34">
         <v>2</v>
@@ -10868,13 +10868,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="35" t="s">
         <v>57</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>58</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -10890,13 +10890,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="35" t="s">
         <v>59</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>60</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -10912,13 +10912,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="35" t="s">
         <v>61</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>62</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -10934,19 +10934,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26">
         <v>4</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" si="0"/>
@@ -10958,13 +10958,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="38" t="s">
         <v>87</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>88</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -10979,13 +10979,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="38" t="s">
         <v>89</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>90</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -11000,13 +11000,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>92</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -11021,13 +11021,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -11043,13 +11043,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -11065,13 +11065,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="38" t="s">
         <v>99</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>100</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -11087,13 +11087,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="38" t="s">
         <v>101</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>102</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -11109,13 +11109,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="38" t="s">
         <v>103</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>104</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -11131,19 +11131,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="38" t="s">
         <v>105</v>
-      </c>
-      <c r="D35" s="38" t="s">
-        <v>106</v>
       </c>
       <c r="E35">
         <v>6</v>
       </c>
       <c r="F35" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G35" s="22" t="str">
         <f t="shared" si="0"/>
@@ -11155,13 +11155,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C36" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="38" t="s">
         <v>107</v>
-      </c>
-      <c r="D36" s="38" t="s">
-        <v>108</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -11177,13 +11177,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C37" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="38" t="s">
         <v>109</v>
-      </c>
-      <c r="D37" s="38" t="s">
-        <v>110</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -11199,13 +11199,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C38" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="38" t="s">
         <v>111</v>
-      </c>
-      <c r="D38" s="38" t="s">
-        <v>112</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -11221,13 +11221,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C39" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="38" t="s">
         <v>113</v>
-      </c>
-      <c r="D39" s="38" t="s">
-        <v>114</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -11243,19 +11243,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C40" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="38" t="s">
         <v>115</v>
-      </c>
-      <c r="D40" s="38" t="s">
-        <v>116</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G40" s="22" t="str">
         <f t="shared" si="0"/>
@@ -11267,13 +11267,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="38" t="s">
         <v>69</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>70</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -11288,13 +11288,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="38" t="s">
         <v>71</v>
-      </c>
-      <c r="D42" s="38" t="s">
-        <v>72</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -11309,13 +11309,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="38" t="s">
         <v>77</v>
-      </c>
-      <c r="D43" s="38" t="s">
-        <v>78</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -11330,13 +11330,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="38" t="s">
         <v>79</v>
-      </c>
-      <c r="D44" s="38" t="s">
-        <v>80</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -11351,13 +11351,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C45" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="38" t="s">
         <v>81</v>
-      </c>
-      <c r="D45" s="38" t="s">
-        <v>82</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -11372,13 +11372,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C46" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="38" t="s">
         <v>83</v>
-      </c>
-      <c r="D46" s="38" t="s">
-        <v>84</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -11393,13 +11393,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C47" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="38" t="s">
         <v>85</v>
-      </c>
-      <c r="D47" s="38" t="s">
-        <v>86</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -11414,13 +11414,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="D48" s="38" t="s">
         <v>175</v>
-      </c>
-      <c r="D48" s="38" t="s">
-        <v>176</v>
       </c>
       <c r="E48" s="40">
         <v>1</v>
@@ -11435,13 +11435,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="38" t="s">
         <v>177</v>
-      </c>
-      <c r="D49" s="38" t="s">
-        <v>178</v>
       </c>
       <c r="E49" s="40">
         <v>2</v>
@@ -11456,13 +11456,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E50" s="34">
         <v>1</v>
@@ -11477,13 +11477,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E51" s="34">
         <v>2</v>
@@ -11498,13 +11498,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C52" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="D52" s="38" t="s">
         <v>224</v>
-      </c>
-      <c r="D52" s="38" t="s">
-        <v>225</v>
       </c>
       <c r="E52" s="40">
         <v>3</v>
@@ -11519,13 +11519,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -11540,13 +11540,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C54" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -11561,13 +11561,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E55" s="36">
         <v>1</v>
@@ -11582,13 +11582,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E56" s="36">
         <v>2</v>
@@ -11603,13 +11603,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C57" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="38" t="s">
         <v>57</v>
-      </c>
-      <c r="D57" s="38" t="s">
-        <v>58</v>
       </c>
       <c r="E57" s="36">
         <v>1</v>
@@ -11624,13 +11624,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="38" t="s">
         <v>59</v>
-      </c>
-      <c r="D58" s="38" t="s">
-        <v>60</v>
       </c>
       <c r="E58" s="36">
         <v>2</v>
@@ -11645,13 +11645,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C59" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" s="38" t="s">
         <v>61</v>
-      </c>
-      <c r="D59" s="38" t="s">
-        <v>62</v>
       </c>
       <c r="E59" s="36">
         <v>3</v>
@@ -11666,19 +11666,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E60" s="36">
         <v>4</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G60" s="22" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update on 30th April after field test
</commit_message>
<xml_diff>
--- a/SpecimenCollectionForm/DB and Documents/Specimen Collection- Endline Parasite.xlsx
+++ b/SpecimenCollectionForm/DB and Documents/Specimen Collection- Endline Parasite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="232">
   <si>
     <t>SLNo</t>
   </si>
@@ -587,9 +587,6 @@
     <t>6.Select the ID of the individual whose sample you are collecting now (select one)</t>
   </si>
   <si>
-    <t>7. Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)</t>
-  </si>
-  <si>
     <t>7.Enter the name of the individual (check against your ID list from Day1 team)</t>
   </si>
   <si>
@@ -696,9 +693,6 @@
   </si>
   <si>
     <t>21.Other: Specify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22. A¨vwbwgqv †U‡÷i djvdj wjLyb </t>
   </si>
   <si>
     <t>22.Enter the result of the anemia test. __ __. __ g/dL</t>
@@ -788,6 +782,15 @@
   </si>
   <si>
     <t xml:space="preserve">4. Date of sample collection </t>
+  </si>
+  <si>
+    <t>tblMainQuesL2</t>
+  </si>
+  <si>
+    <t>7.AvBwW Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)</t>
+  </si>
+  <si>
+    <t>22. A¨vwbwgqv †U‡÷i djvdj wjLyb. di‡gU: `yB wWwRU Gi ci `kwg‡Ki ci GK wWwRU</t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DK440"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <selection activeCell="V2" sqref="V2:V33"/>
     </sheetView>
   </sheetViews>
@@ -1871,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>46</v>
@@ -1880,10 +1883,10 @@
         <v>27</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>26</v>
@@ -2010,7 +2013,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H5" s="29" t="s">
         <v>34</v>
@@ -2145,10 +2148,10 @@
         <v>142</v>
       </c>
       <c r="E8" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>170</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>171</v>
       </c>
       <c r="H8" s="29" t="s">
         <v>47</v>
@@ -2174,7 +2177,7 @@
       <c r="U8" s="40"/>
       <c r="V8" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'q7','frmtext', 'tblMainQuesL','7. Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)','7.Enter the name of the individual (check against your ID list from Day1 team)','','q8','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'q7','frmtext', 'tblMainQuesL','7.AvBwW Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)','7.Enter the name of the individual (check against your ID list from Day1 team)','','q8','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="9" spans="1:115" s="40" customFormat="1" ht="90.75">
@@ -2191,10 +2194,10 @@
         <v>142</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H9" s="29" t="s">
         <v>49</v>
@@ -2224,7 +2227,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>50</v>
@@ -2256,7 +2259,7 @@
       <c r="U10" s="40"/>
       <c r="V10" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'q9','frmsinglechoice', 'tblMainQuesL','9.D³ e¨w³ †_‡K gj/cvqLvbvi bgybv msMÖn Kiv n‡q‡Q wK?','9.Has a stool sample been collected from this individual?','','q10','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'q9','frmsinglechoice', 'tblMainQuesL2','9.D³ e¨w³ †_‡K gj/cvqLvbvi bgybv msMÖn Kiv n‡q‡Q wK?','9.Has a stool sample been collected from this individual?','','q10','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="11" spans="1:115" ht="90">
@@ -2270,7 +2273,7 @@
         <v>46</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E11" s="27" t="s">
         <v>54</v>
@@ -2302,7 +2305,7 @@
       <c r="U11" s="40"/>
       <c r="V11" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('10', 'q10','frmsinglechoice', 'tblMainQuesL','10.‡Kb cvqLvbvi bgybv msMÖn Kiv hvqwb?','10.Why has a stool sample not been collected?  ','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('10', 'q10','frmsinglechoice', 'tblMainQuesL2','10.‡Kb cvqLvbvi bgybv msMÖn Kiv hvqwb?','10.Why has a stool sample not been collected?  ','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="12" spans="1:115" s="40" customFormat="1" ht="90.75">
@@ -2310,19 +2313,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>159</v>
@@ -2338,7 +2341,7 @@
       </c>
       <c r="V12" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('11', 'q10_other','frmtext', 'tblMainQuesL','10.Ab¨vY¨t wbw`©ó K‡i wjLyb','10.Other: Specify','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('11', 'q10_other','frmtext', 'tblMainQuesL2','10.Ab¨vY¨t wbw`©ó K‡i wjLyb','10.Other: Specify','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="13" spans="1:115" s="40" customFormat="1" ht="105">
@@ -2352,10 +2355,10 @@
         <v>155</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>157</v>
@@ -2374,7 +2377,7 @@
       </c>
       <c r="V13" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('12', 'msg01','frmmessage', 'tblMainQues','D³ LvbvwU bZzb BB wm‡½j Av‡g©i AšÍ©fz³ wn‡m‡e wb‡`©k Ki‡Z ev †evSv‡Z msMÖnK…Z ÷zj K‡›UBbv‡ii wQwci Dci ZviKv wPý (*) emvb','NOTE: Mark the cap of the stool collection containersin this household with * to show that this household is in the single arm EE cohort.','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('12', 'msg01','frmmessage', 'tblMainQuesL2','D³ LvbvwU bZzb BB wm‡½j Av‡g©i AšÍ©fz³ wn‡m‡e wb‡`©k Ki‡Z ev †evSv‡Z msMÖnK…Z ÷zj K‡›UBbv‡ii wQwci Dci ZviKv wPý (*) emvb','NOTE: Mark the cap of the stool collection containersin this household with * to show that this household is in the single arm EE cohort.','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="14" spans="1:115" ht="157.5">
@@ -2388,13 +2391,13 @@
         <v>155</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E14" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" s="26" t="s">
         <v>180</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>181</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>52</v>
@@ -2420,7 +2423,7 @@
       <c r="U14" s="40"/>
       <c r="V14" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('13', 'msg02','frmmessage', 'tblMainQuesL','wbwðZ Kiæb †h cvqLvbvi bgybv cixÿv Kivi Rb¨ Avcwb K¨v‡Uv-K¨vUR GwjKU ˆZix K‡i‡Qb Ges K¨v‡Uv-K¨vUR GwjK‡Ui Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q| ','Make sure that you have prepared a Kato-Katz aliquot for this individual and make sure that the sample ID and random ID of the barcode on the Kato-Katz aliquot match the following:','','q11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('13', 'msg02','frmmessage', 'tblMainQuesL2','wbwðZ Kiæb †h cvqLvbvi bgybv cixÿv Kivi Rb¨ Avcwb K¨v‡Uv-K¨vUR GwjKU ˆZix K‡i‡Qb Ges K¨v‡Uv-K¨vUR GwjK‡Ui Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q| ','Make sure that you have prepared a Kato-Katz aliquot for this individual and make sure that the sample ID and random ID of the barcode on the Kato-Katz aliquot match the following:','','q11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="15" spans="1:115" ht="90">
@@ -2434,13 +2437,13 @@
         <v>66</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E15" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15" s="26" t="s">
         <v>182</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>183</v>
       </c>
       <c r="H15" s="29" t="s">
         <v>65</v>
@@ -2466,7 +2469,7 @@
       <c r="U15" s="40"/>
       <c r="V15" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('14', 'q11','frmyeartomin', 'tblMainQuesL','11.msM„nxZ bgybv Kyje†· ivLvi ïiæi mgqUv wjwce× Kiæb (24 N›Uv wnmv‡e)','11.Enter the cold chain start time  (24-hr scale)','','q12','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('14', 'q11','frmyeartomin', 'tblMainQuesL2','11.msM„nxZ bgybv Kyje†· ivLvi ïiæi mgqUv wjwce× Kiæb (24 N›Uv wnmv‡e)','11.Enter the cold chain start time  (24-hr scale)','','q12','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="16" spans="1:115" ht="90">
@@ -2480,13 +2483,13 @@
         <v>46</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E16" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>184</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>185</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>67</v>
@@ -2512,7 +2515,7 @@
       <c r="U16" s="40"/>
       <c r="V16" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('15', 'q12','frmsinglechoice', 'tblMainQuesL','12.(পর্যবেক্ষন করুন) cvqLvbvi aib †Kgb?','12.(obs) Stool consistency','','q13','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('15', 'q12','frmsinglechoice', 'tblMainQuesL2','12.(পর্যবেক্ষন করুন) cvqLvbvi aib †Kgb?','12.(obs) Stool consistency','','q13','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="90">
@@ -2526,13 +2529,13 @@
         <v>46</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E17" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>186</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>187</v>
       </c>
       <c r="H17" s="29" t="s">
         <v>72</v>
@@ -2558,7 +2561,7 @@
       <c r="U17" s="40"/>
       <c r="V17" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('16', 'q13','frmsinglechoice', 'tblMainQuesL','13.(পর্যবেক্ষন করুন) cvqLvbvi eb© wK?','13. (obs) Stool color','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('16', 'q13','frmsinglechoice', 'tblMainQuesL2','13.(পর্যবেক্ষন করুন) cvqLvbvi eb© wK?','13. (obs) Stool color','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="90.75">
@@ -2572,13 +2575,13 @@
         <v>48</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E18" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>188</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>189</v>
       </c>
       <c r="H18" s="29" t="s">
         <v>72</v>
@@ -2604,7 +2607,7 @@
       <c r="U18" s="40"/>
       <c r="V18" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('17', 'q13_other','frmtext', 'tblMainQuesL','13.Ab¨vY¨t wbw`©ó K‡i wjLyb','13.Other: Specify','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('17', 'q13_other','frmtext', 'tblMainQuesL2','13.Ab¨vY¨t wbw`©ó K‡i wjLyb','13.Other: Specify','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="90">
@@ -2618,13 +2621,13 @@
         <v>35</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E19" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>191</v>
       </c>
       <c r="H19" s="29" t="s">
         <v>73</v>
@@ -2650,7 +2653,7 @@
       <c r="U19" s="40"/>
       <c r="V19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('18', 'q14','frmmultiplechoice', 'tblMainQuesL','14. (পর্যবেক্ষন করুন) msM„nxZ cvqLvbvi bgybvi g‡a¨ A¯^vfvweK wKQz †`Lv †M‡Q wK? (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','14.(obs) Do you see any abnormal characteristics of the collected stool sample? (Select all that apply)','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('18', 'q14','frmmultiplechoice', 'tblMainQuesL2','14. (পর্যবেক্ষন করুন) msM„nxZ cvqLvbvi bgybvi g‡a¨ A¯^vfvweK wKQz †`Lv †M‡Q wK? (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','14.(obs) Do you see any abnormal characteristics of the collected stool sample? (Select all that apply)','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="90.75">
@@ -2664,13 +2667,13 @@
         <v>48</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E20" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>192</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>193</v>
       </c>
       <c r="G20" s="36"/>
       <c r="H20" s="29" t="s">
@@ -2697,7 +2700,7 @@
       <c r="U20" s="40"/>
       <c r="V20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('19', 'q14_other','frmtext', 'tblMainQuesL','14.Ab¨vY¨t wbw`©ó K‡i wjLyb','14.Other: Specify','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('19', 'q14_other','frmtext', 'tblMainQuesL2','14.Ab¨vY¨t wbw`©ó K‡i wjLyb','14.Other: Specify','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="90">
@@ -2711,13 +2714,13 @@
         <v>46</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E21" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H21" s="29" t="s">
         <v>75</v>
@@ -2743,7 +2746,7 @@
       <c r="U21" s="40"/>
       <c r="V21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('20', 'q15','frmsinglechoice', 'tblMainQuesL','15.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','15.Enter the day of defecation','','q16','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('20', 'q15','frmsinglechoice', 'tblMainQuesL2','15.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','15.Enter the day of defecation','','q16','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="90">
@@ -2757,13 +2760,13 @@
         <v>66</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E22" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="F22" s="28" t="s">
         <v>195</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>196</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>93</v>
@@ -2789,7 +2792,7 @@
       <c r="U22" s="40"/>
       <c r="V22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('21', 'q16','frmyeartomin', 'tblMainQuesL','16.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi mgq wjwce× Kiæb (24 N›Uv wnmv‡e, Rvwb bv n‡j 99:99 emvb)','16.Enter the time of defecation (24-hr scale, enter 99:99 for DK)','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('21', 'q16','frmyeartomin', 'tblMainQuesL2','16.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi mgq wjwce× Kiæb (24 N›Uv wnmv‡e, Rvwb bv n‡j 99:99 emvb)','16.Enter the time of defecation (24-hr scale, enter 99:99 for DK)','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="90">
@@ -2803,13 +2806,13 @@
         <v>46</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E23" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="F23" s="26" t="s">
         <v>197</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>198</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>93</v>
@@ -2835,7 +2838,7 @@
       <c r="U23" s="40"/>
       <c r="V23" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('22', 'q17','frmsinglechoice', 'tblMainQuesL','17.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','17.Enter the approximate time of defecation','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('22', 'q17','frmsinglechoice', 'tblMainQuesL2','17.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','17.Enter the approximate time of defecation','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="24" spans="1:22" s="40" customFormat="1" ht="90">
@@ -2849,13 +2852,13 @@
         <v>46</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E24" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F24" s="28" t="s">
         <v>199</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>200</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>166</v>
@@ -2871,7 +2874,7 @@
       </c>
       <c r="V24" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('23', 'q18','frmsinglechoice', 'tblMainQuesL','18.cvqLvbvi bgybvwU GKev‡I Kiv cvqLvbv †_‡K bvwKGKvwaKevi Kiv cvqLvbv †_‡K msMÖn Kiv n‡q‡Q?','18.Was the stool collected from one defecation event or multiple defecation events?','','q19a','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('23', 'q18','frmsinglechoice', 'tblMainQuesL2','18.cvqLvbvi bgybvwU GKev‡I Kiv cvqLvbv †_‡K bvwKGKvwaKevi Kiv cvqLvbv †_‡K msMÖn Kiv n‡q‡Q?','18.Was the stool collected from one defecation event or multiple defecation events?','','q19a','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="90">
@@ -2885,13 +2888,13 @@
         <v>46</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E25" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="26" t="s">
         <v>201</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>202</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>167</v>
@@ -2917,7 +2920,7 @@
       <c r="U25" s="40"/>
       <c r="V25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('24', 'q19a','frmsinglechoice', 'tblMainQuesL','19.K.(পর্যবেক্ষন করুন) D³ e¨w³/wkï cv‡q RyZv c‡o‡Q wK ?','19.a. (obs) Is the individual wearing shoes? ','','q19b','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('24', 'q19a','frmsinglechoice', 'tblMainQuesL2','19.K.(পর্যবেক্ষন করুন) D³ e¨w³/wkï cv‡q RyZv c‡o‡Q wK ?','19.a. (obs) Is the individual wearing shoes? ','','q19b','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="26" spans="1:22" s="40" customFormat="1" ht="90">
@@ -2931,13 +2934,13 @@
         <v>46</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E26" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" s="47" t="s">
         <v>203</v>
-      </c>
-      <c r="F26" s="47" t="s">
-        <v>204</v>
       </c>
       <c r="H26" s="29" t="s">
         <v>162</v>
@@ -2953,7 +2956,7 @@
       </c>
       <c r="V26" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('25', 'q19b','frmsinglechoice', 'tblMainQuesL','19.L.BB wUg D³ Uv‡M©U wkï (Ges Uv‡M©U wkïi RgR) †_‡K i‡³i bgybv msMÖn K‡i‡Q wK ? ','19.b. Has a target child (and twin) blood sample already been collected by the EE team? ','','msg03','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('25', 'q19b','frmsinglechoice', 'tblMainQuesL2','19.L.BB wUg D³ Uv‡M©U wkï (Ges Uv‡M©U wkïi RgR) †_‡K i‡³i bgybv msMÖn K‡i‡Q wK ? ','19.b. Has a target child (and twin) blood sample already been collected by the EE team? ','','msg03','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="27" spans="1:22" s="40" customFormat="1" ht="90">
@@ -2967,7 +2970,7 @@
         <v>155</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E27" s="31" t="s">
         <v>163</v>
@@ -2989,7 +2992,7 @@
       </c>
       <c r="V27" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('26', 'msg03','frmmessage', 'tblMainQuesL','D³ Lvbvi Uv‡M©U wkï Ges Uv‡M©U wkïi RgR †_‡K i‡³i bgybv msMÖn Ki‡Z n‡ebv|','Do not collect a blood sample from target child (and twin) in this household','','q20','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('26', 'msg03','frmmessage', 'tblMainQuesL2','D³ Lvbvi Uv‡M©U wkï Ges Uv‡M©U wkïi RgR †_‡K i‡³i bgybv msMÖn Ki‡Z n‡ebv|','Do not collect a blood sample from target child (and twin) in this household','','q20','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="90">
@@ -3003,13 +3006,13 @@
         <v>46</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E28" s="27" t="s">
         <v>117</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>116</v>
@@ -3035,7 +3038,7 @@
       <c r="U28" s="40"/>
       <c r="V28" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('27', 'q20','frmsinglechoice', 'tblMainQuesL','20.D³ e¨w³/ wkï †_‡K i‡³i bgybv msMÖn Kiv n‡q‡Q wK?','20.Has a blood sample been collected from this individual?','','q21','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('27', 'q20','frmsinglechoice', 'tblMainQuesL2','20.D³ e¨w³/ wkï †_‡K i‡³i bgybv msMÖn Kiv n‡q‡Q wK?','20.Has a blood sample been collected from this individual?','','q21','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="90">
@@ -3049,7 +3052,7 @@
         <v>46</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E29" s="27" t="s">
         <v>119</v>
@@ -3081,7 +3084,7 @@
       <c r="U29" s="40"/>
       <c r="V29" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('28', 'q21','frmsinglechoice', 'tblMainQuesL','21.‡Kb i‡³i bgybv msMÖn Kiv hvqwb?','21.Why has a blood sample not been collected?','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('28', 'q21','frmsinglechoice', 'tblMainQuesL2','21.‡Kb i‡³i bgybv msMÖn Kiv hvqwb?','21.Why has a blood sample not been collected?','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="30" spans="1:22" s="40" customFormat="1" ht="90.75">
@@ -3089,19 +3092,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C30" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E30" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="26" t="s">
         <v>205</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>206</v>
       </c>
       <c r="H30" s="29" t="s">
         <v>118</v>
@@ -3117,7 +3120,7 @@
       </c>
       <c r="V30" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('29', 'q21_other','frmtext', 'tblMainQuesL','21.Ab¨vY¨t wbw`©ó K‡i wjLyb','21.Other: Specify','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('29', 'q21_other','frmtext', 'tblMainQuesL2','21.Ab¨vY¨t wbw`©ó K‡i wjLyb','21.Other: Specify','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="90">
@@ -3131,13 +3134,13 @@
         <v>124</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H31" s="29" t="s">
         <v>165</v>
@@ -3163,7 +3166,7 @@
       <c r="U31" s="40"/>
       <c r="V31" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('30', 'q22','frmnumeric', 'tblMainQuesL','22. A¨vwbwgqv †U‡÷i djvdj wjLyb ','22.Enter the result of the anemia test. __ __. __ g/dL','','msg04','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('30', 'q22','frmnumeric', 'tblMainQuesL2','22. A¨vwbwgqv †U‡÷i djvdj wjLyb. di‡gU: `yB wWwRU Gi ci `kwg‡Ki ci GK wWwRU','22.Enter the result of the anemia test. __ __. __ g/dL','','msg04','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="115.5">
@@ -3177,13 +3180,13 @@
         <v>155</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H32" s="29" t="s">
         <v>121</v>
@@ -3209,7 +3212,7 @@
       <c r="U32" s="40"/>
       <c r="V32" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('31', 'msg04','frmmessage', 'tblMainQuesL','wbwðZ Kiæb eøvW ¯úU wdëvi †ccv‡ii Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q|','Make sure that the sample ID and random ID of the barcode on the blood spot filter paper match the following:','','q23','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('31', 'msg04','frmmessage', 'tblMainQuesL2','wbwðZ Kiæb eøvW ¯úU wdëvi †ccv‡ii Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q|','Make sure that the sample ID and random ID of the barcode on the blood spot filter paper match the following:','','q23','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="90">
@@ -3223,7 +3226,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="E33" s="27" t="s">
         <v>122</v>
@@ -3253,7 +3256,7 @@
       <c r="U33" s="40"/>
       <c r="V33" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('32', 'q23','frmnumeric', 'tblMainQuesL','23.wdëvi †ccv‡i i‡³i Kq‡dvUv bgybv msMÖn Kiv n‡q‡Q Zvi msL¨v wjLyb (msL¨v 1 †_‡K 6 Gi g‡a¨ n‡e)','23.Enter the number of spots filled (has to be between 1 and 6)','','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('32', 'q23','frmnumeric', 'tblMainQuesL2','23.wdëvi †ccv‡i i‡³i Kq‡dvUv bgybv msMÖn Kiv n‡q‡Q Zvi msL¨v wjLyb (msL¨v 1 †_‡K 6 Gi g‡a¨ n‡e)','23.Enter the number of spots filled (has to be between 1 and 6)','','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="45" spans="1:22">
@@ -10379,7 +10382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G60"/>
     </sheetView>
   </sheetViews>
@@ -10422,7 +10425,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>44</v>
@@ -10443,7 +10446,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>45</v>
@@ -10762,10 +10765,10 @@
         <v>47</v>
       </c>
       <c r="C18" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="40" t="s">
         <v>172</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>173</v>
       </c>
       <c r="E18" s="42">
         <v>1</v>
@@ -10783,10 +10786,10 @@
         <v>47</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E19" s="42">
         <v>2</v>
@@ -10804,7 +10807,7 @@
         <v>47</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>111</v>
@@ -10946,7 +10949,7 @@
         <v>4</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" si="0"/>
@@ -11155,7 +11158,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C36" s="41" t="s">
         <v>106</v>
@@ -11177,7 +11180,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C37" s="41" t="s">
         <v>108</v>
@@ -11199,7 +11202,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C38" s="41" t="s">
         <v>110</v>
@@ -11221,7 +11224,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C39" s="41" t="s">
         <v>112</v>
@@ -11243,7 +11246,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C40" s="41" t="s">
         <v>114</v>
@@ -11417,10 +11420,10 @@
         <v>93</v>
       </c>
       <c r="C48" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" s="38" t="s">
         <v>174</v>
-      </c>
-      <c r="D48" s="38" t="s">
-        <v>175</v>
       </c>
       <c r="E48" s="40">
         <v>1</v>
@@ -11438,10 +11441,10 @@
         <v>93</v>
       </c>
       <c r="C49" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="D49" s="38" t="s">
         <v>176</v>
-      </c>
-      <c r="D49" s="38" t="s">
-        <v>177</v>
       </c>
       <c r="E49" s="40">
         <v>2</v>
@@ -11501,10 +11504,10 @@
         <v>166</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E52" s="40">
         <v>3</v>
@@ -11678,7 +11681,7 @@
         <v>4</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G60" s="22" t="str">
         <f t="shared" si="0"/>

</xml_diff>